<commit_message>
Added dropdowns for wash and resus volumes
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6E74EE-C03F-471B-B267-9DD7016E8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92A6517-4EC1-4A69-B868-3F30AA622A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="442">
   <si>
     <t>Date:</t>
   </si>
@@ -1719,6 +1719,24 @@
       </rPr>
       <t>Combine equal volume of all samples into a new LoBind tube</t>
     </r>
+  </si>
+  <si>
+    <t>Ento</t>
+  </si>
+  <si>
+    <t>Applies to</t>
+  </si>
+  <si>
+    <t>Resuspension Vol (ul)</t>
+  </si>
+  <si>
+    <t>Wash Volume (ul)</t>
+  </si>
+  <si>
+    <t>Plasmo</t>
+  </si>
+  <si>
+    <t>Plasmodium</t>
   </si>
 </sst>
 </file>
@@ -2583,37 +2601,107 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2628,95 +2716,25 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -3794,8 +3812,8 @@
   </sheetPr>
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3804,175 +3822,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="130" t="s">
         <v>395</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="97"/>
-      <c r="J2" s="98" t="s">
+      <c r="H2" s="113"/>
+      <c r="J2" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="98"/>
+      <c r="K2" s="132"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="100"/>
+      <c r="K3" s="134"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="101" t="s">
+      <c r="J4" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="101"/>
+      <c r="K4" s="135"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="103" t="str">
+      <c r="B5" s="125"/>
+      <c r="C5" s="109" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="104"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="105" t="str">
+      <c r="B6" s="125"/>
+      <c r="C6" s="127" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="109" t="str">
+      <c r="B9" s="120"/>
+      <c r="C9" s="121" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="109" t="str">
+      <c r="B10" s="120"/>
+      <c r="C10" s="121" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
+      <c r="A11" s="94" t="s">
         <v>423</v>
       </c>
-      <c r="B11" s="95"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
+      <c r="F11" s="124"/>
       <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
@@ -3980,10 +3998,10 @@
       <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="95" t="s">
+      <c r="A12" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="95"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="27"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -3991,32 +4009,32 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="122"/>
+      <c r="K14" s="122"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="6"/>
@@ -4027,11 +4045,11 @@
       </c>
       <c r="C16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="I16" s="111" t="s">
+      <c r="I16" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
+      <c r="J16" s="123"/>
+      <c r="K16" s="123"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -4061,119 +4079,119 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112" t="s">
+      <c r="A19" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="113" t="s">
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113" t="str">
+      <c r="E19" s="119"/>
+      <c r="F19" s="119" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G19" s="113"/>
-      <c r="I19" s="114" t="s">
+      <c r="G19" s="119"/>
+      <c r="I19" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="114"/>
+      <c r="J19" s="98"/>
       <c r="K19" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="117" t="s">
+      <c r="B20" s="102"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="118" t="s">
+      <c r="E20" s="114"/>
+      <c r="F20" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="118"/>
-      <c r="I20" s="119">
+      <c r="G20" s="115"/>
+      <c r="I20" s="107">
         <v>20</v>
       </c>
-      <c r="J20" s="119"/>
+      <c r="J20" s="107"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="117" t="str">
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="114" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E21" s="117"/>
-      <c r="F21" s="118" t="s">
+      <c r="E21" s="114"/>
+      <c r="F21" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="118"/>
-      <c r="I21" s="119">
+      <c r="G21" s="115"/>
+      <c r="I21" s="107">
         <v>65</v>
       </c>
-      <c r="J21" s="119"/>
+      <c r="J21" s="107"/>
       <c r="K21" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="120">
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="117">
         <v>1.4</v>
       </c>
-      <c r="E22" s="120"/>
-      <c r="F22" s="118">
+      <c r="E22" s="117"/>
+      <c r="F22" s="115">
         <f>SUM(D22*exp_rxns*(1+$D$18))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="118"/>
-      <c r="I22" s="119">
+      <c r="G22" s="115"/>
+      <c r="I22" s="107">
         <v>4</v>
       </c>
-      <c r="J22" s="119"/>
+      <c r="J22" s="107"/>
       <c r="K22" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="120">
+      <c r="B23" s="102"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="117">
         <v>0.6</v>
       </c>
-      <c r="E23" s="120"/>
-      <c r="F23" s="118">
+      <c r="E23" s="117"/>
+      <c r="F23" s="115">
         <f>SUM(D23*exp_rxns*(1+$D$18))</f>
         <v>0</v>
       </c>
-      <c r="G23" s="118"/>
+      <c r="G23" s="115"/>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="D24" s="121">
+      <c r="D24" s="118">
         <f>SUM(D22:D23)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E24" s="121"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D22:D23)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -4198,103 +4216,103 @@
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="112" t="s">
+      <c r="A27" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113" t="s">
+      <c r="B27" s="104"/>
+      <c r="C27" s="104"/>
+      <c r="D27" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113" t="str">
+      <c r="E27" s="119"/>
+      <c r="F27" s="119" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G27" s="113"/>
-      <c r="I27" s="114" t="s">
+      <c r="G27" s="119"/>
+      <c r="I27" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="114"/>
+      <c r="J27" s="98"/>
       <c r="K27" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117">
+      <c r="B28" s="102"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="114">
         <v>0.5</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="118" t="s">
+      <c r="E28" s="114"/>
+      <c r="F28" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="118"/>
-      <c r="I28" s="119">
+      <c r="G28" s="115"/>
+      <c r="I28" s="107">
         <v>20</v>
       </c>
-      <c r="J28" s="119"/>
+      <c r="J28" s="107"/>
       <c r="K28" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117">
+      <c r="B29" s="102"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="114">
         <v>6</v>
       </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="118">
+      <c r="E29" s="114"/>
+      <c r="F29" s="115">
         <f>SUM(D29*exp_rxns*(1+$D$26))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="118"/>
-      <c r="I29" s="119">
+      <c r="G29" s="115"/>
+      <c r="I29" s="107">
         <v>65</v>
       </c>
-      <c r="J29" s="119"/>
+      <c r="J29" s="107"/>
       <c r="K29" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="117">
+      <c r="B30" s="102"/>
+      <c r="C30" s="102"/>
+      <c r="D30" s="114">
         <v>0.2</v>
       </c>
-      <c r="E30" s="117"/>
-      <c r="F30" s="118">
+      <c r="E30" s="114"/>
+      <c r="F30" s="115">
         <f>SUM(D30*exp_rxns*(1+$D$26))</f>
         <v>0</v>
       </c>
-      <c r="G30" s="118"/>
-      <c r="I30" s="119">
+      <c r="G30" s="115"/>
+      <c r="I30" s="107">
         <v>8</v>
       </c>
-      <c r="J30" s="119"/>
+      <c r="J30" s="107"/>
       <c r="K30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="D31" s="122">
+      <c r="D31" s="116">
         <f>SUM(D28:D30)+D24</f>
         <v>18.7</v>
       </c>
-      <c r="E31" s="122"/>
+      <c r="E31" s="116"/>
       <c r="F31" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D29:D30)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -4358,19 +4376,19 @@
       <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="127" t="s">
+      <c r="A37" s="112" t="s">
         <v>434</v>
       </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="97"/>
-      <c r="K37" s="97"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="113"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="71" t="s">
@@ -4393,10 +4411,10 @@
       <c r="C39" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D39" s="123" t="s">
+      <c r="D39" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="123"/>
+      <c r="E39" s="100"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
@@ -4405,11 +4423,11 @@
       </c>
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
-      <c r="D40" s="124">
+      <c r="D40" s="111">
         <f>SUM(B40*C40)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="124"/>
+      <c r="E40" s="111"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -4433,97 +4451,97 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="114" t="s">
+      <c r="A44" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="125" t="s">
+      <c r="B44" s="98"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="125"/>
-      <c r="I44" s="114" t="s">
+      <c r="E44" s="99"/>
+      <c r="I44" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="J44" s="114"/>
+      <c r="J44" s="98"/>
       <c r="K44" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="126">
+      <c r="B45" s="102"/>
+      <c r="C45" s="102"/>
+      <c r="D45" s="101">
         <f>IF(B40="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D40)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D40)))</f>
         <v>30</v>
       </c>
-      <c r="E45" s="126"/>
+      <c r="E45" s="101"/>
       <c r="F45" s="5"/>
-      <c r="I45" s="119" t="s">
+      <c r="I45" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="J45" s="119"/>
+      <c r="J45" s="107"/>
       <c r="K45" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="116" t="s">
+      <c r="A46" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="126">
+      <c r="B46" s="102"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="101">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D45),"")</f>
         <v>0</v>
       </c>
-      <c r="E46" s="126"/>
+      <c r="E46" s="101"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="116" t="s">
+      <c r="A47" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="103">
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="109">
         <v>5</v>
       </c>
-      <c r="E47" s="103"/>
+      <c r="E47" s="109"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="102" t="s">
         <v>388</v>
       </c>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="103">
+      <c r="B48" s="102"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="109">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E48" s="103"/>
+      <c r="E48" s="109"/>
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="116" t="s">
+      <c r="A49" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="103">
+      <c r="B49" s="102"/>
+      <c r="C49" s="102"/>
+      <c r="D49" s="109">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E49" s="103"/>
+      <c r="E49" s="109"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D50" s="128">
+      <c r="D50" s="110">
         <f>SUM(D45:D49)</f>
         <v>50</v>
       </c>
-      <c r="E50" s="128"/>
+      <c r="E50" s="110"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -4540,20 +4558,20 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="131" t="s">
+      <c r="A54" s="108" t="s">
         <v>391</v>
       </c>
-      <c r="B54" s="131"/>
-      <c r="C54" s="131"/>
-      <c r="D54" s="131"/>
-      <c r="E54" s="131"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="131"/>
-      <c r="I54" s="131"/>
-      <c r="J54" s="131"/>
-      <c r="K54" s="131"/>
-      <c r="L54" s="131"/>
+      <c r="B54" s="108"/>
+      <c r="C54" s="108"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="108"/>
+      <c r="H54" s="108"/>
+      <c r="I54" s="108"/>
+      <c r="J54" s="108"/>
+      <c r="K54" s="108"/>
+      <c r="L54" s="108"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="71" t="s">
@@ -4571,38 +4589,38 @@
       <c r="L55" s="88"/>
     </row>
     <row r="56" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="112" t="s">
+      <c r="A56" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="112"/>
-      <c r="C56" s="112" t="s">
+      <c r="B56" s="104"/>
+      <c r="C56" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112" t="s">
+      <c r="D56" s="104"/>
+      <c r="E56" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112" t="s">
+      <c r="F56" s="104"/>
+      <c r="G56" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="H56" s="112"/>
+      <c r="H56" s="104"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="129">
+      <c r="A57" s="105">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B57" s="129"/>
-      <c r="C57" s="130"/>
-      <c r="D57" s="130"/>
-      <c r="E57" s="130"/>
-      <c r="F57" s="130"/>
-      <c r="G57" s="119">
+      <c r="B57" s="105"/>
+      <c r="C57" s="106"/>
+      <c r="D57" s="106"/>
+      <c r="E57" s="106"/>
+      <c r="F57" s="106"/>
+      <c r="G57" s="107">
         <f>SUM(C57*E57)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="119"/>
+      <c r="H57" s="107"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -4621,61 +4639,61 @@
       <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="114" t="s">
+      <c r="A61" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="114"/>
-      <c r="C61" s="114"/>
-      <c r="D61" s="125" t="s">
+      <c r="B61" s="98"/>
+      <c r="C61" s="98"/>
+      <c r="D61" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E61" s="125"/>
+      <c r="E61" s="99"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="123" t="s">
+      <c r="A62" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="123"/>
-      <c r="C62" s="123"/>
-      <c r="D62" s="126">
+      <c r="B62" s="100"/>
+      <c r="C62" s="100"/>
+      <c r="D62" s="101">
         <f>IF(C57="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G57)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G57)))</f>
         <v>12</v>
       </c>
-      <c r="E62" s="126"/>
+      <c r="E62" s="101"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="123" t="s">
+      <c r="A63" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="123"/>
-      <c r="C63" s="123"/>
-      <c r="D63" s="126" t="str">
+      <c r="B63" s="100"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="101" t="str">
         <f>IFERROR((IF(SUM(12-D62)=0,"-",SUM(12-D62))),"")</f>
         <v>-</v>
       </c>
-      <c r="E63" s="126"/>
+      <c r="E63" s="101"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="116" t="s">
+      <c r="A64" s="102" t="s">
         <v>396</v>
       </c>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="132">
+      <c r="B64" s="102"/>
+      <c r="C64" s="102"/>
+      <c r="D64" s="103">
         <v>37.5</v>
       </c>
-      <c r="E64" s="132"/>
+      <c r="E64" s="103"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="116" t="s">
+      <c r="A65" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="B65" s="116"/>
-      <c r="C65" s="116"/>
-      <c r="D65" s="132">
+      <c r="B65" s="102"/>
+      <c r="C65" s="102"/>
+      <c r="D65" s="103">
         <v>25.5</v>
       </c>
-      <c r="E65" s="132"/>
+      <c r="E65" s="103"/>
       <c r="F65" s="5" t="s">
         <v>55</v>
       </c>
@@ -4687,75 +4705,75 @@
       <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="95" t="s">
+      <c r="A68" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="B68" s="95"/>
-      <c r="C68" s="134"/>
-      <c r="D68" s="134"/>
+      <c r="B68" s="94"/>
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
       <c r="E68" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="95" t="s">
+      <c r="A69" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="133"/>
-      <c r="D69" s="133"/>
+      <c r="B69" s="94"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="95"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="95" t="s">
+      <c r="A70" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="95"/>
-      <c r="C70" s="133"/>
-      <c r="D70" s="133"/>
+      <c r="B70" s="94"/>
+      <c r="C70" s="95"/>
+      <c r="D70" s="95"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="95" t="s">
+      <c r="A71" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="95"/>
-      <c r="C71" s="135" t="str">
+      <c r="B71" s="94"/>
+      <c r="C71" s="97" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D71" s="135"/>
+      <c r="D71" s="97"/>
       <c r="E71" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="95" t="s">
+      <c r="A72" s="94" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="95"/>
-      <c r="C72" s="134"/>
-      <c r="D72" s="134"/>
+      <c r="B72" s="94"/>
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
       <c r="E72" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="95" t="s">
+      <c r="A73" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="95"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="133"/>
+      <c r="B73" s="94"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
       <c r="E73" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="95" t="s">
+      <c r="A74" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="95"/>
-      <c r="C74" s="133"/>
-      <c r="D74" s="133"/>
+      <c r="B74" s="94"/>
+      <c r="C74" s="95"/>
+      <c r="D74" s="95"/>
       <c r="E74" s="9" t="s">
         <v>68</v>
       </c>
@@ -4763,6 +4781,110 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="118">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:K14"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="D65:E65"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="C73:D73"/>
     <mergeCell ref="A74:B74"/>
@@ -4777,110 +4899,6 @@
     <mergeCell ref="C71:D71"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A54:L54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="A35">
     <cfRule type="expression" dxfId="14" priority="5">
@@ -4979,7 +4997,7 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>reference!$E$3:$E$4</xm:f>
@@ -5025,6 +5043,18 @@
           </x14:formula2>
           <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{18233F5E-F0C9-4D48-8942-CE3D9609CBE0}">
+          <x14:formula1>
+            <xm:f>reference!$E$38:$E$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>F35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8AB4769-634A-4E55-85CA-F2BAE73B69BB}">
+          <x14:formula1>
+            <xm:f>reference!$E$42:$E$43</xm:f>
+          </x14:formula1>
+          <xm:sqref>G35</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -15121,10 +15151,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15498,8 +15528,56 @@
         <v>402</v>
       </c>
     </row>
+    <row r="37" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="83" t="s">
+        <v>439</v>
+      </c>
+      <c r="F37" s="80" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="47">
+        <v>700</v>
+      </c>
+      <c r="F38" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="47">
+        <v>200</v>
+      </c>
+      <c r="F39" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="83" t="s">
+        <v>438</v>
+      </c>
+      <c r="F41" s="80" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="47">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="47">
+        <v>70</v>
+      </c>
+      <c r="F43" t="s">
+        <v>441</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
       <formula1>$E$23:$E$30</formula1>
@@ -15995,9 +16073,7 @@
   </sheetPr>
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Updated templates, example data to and processing of filled templates
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8CCCE9-79EB-45DA-B82E-0AB109BA2E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5174F1E2-3485-4463-89C4-4752D2F4523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29625" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,31 +22,31 @@
   </sheets>
   <definedNames>
     <definedName name="adaptlig_dna_maxvol">reference!$B$4</definedName>
-    <definedName name="adaptlig_rxn_vol">Assay!$F$43</definedName>
-    <definedName name="adaptlig_targetmass">Assay!$B$43</definedName>
-    <definedName name="DNAconc_library">Assay!$G$57</definedName>
-    <definedName name="DNAconc_pooled">Assay!$D$40</definedName>
+    <definedName name="adaptlig_rxn_vol">Assay!$F$42</definedName>
+    <definedName name="adaptlig_targetmass">Assay!$B$42</definedName>
+    <definedName name="DNAconc_library">Assay!$G$56</definedName>
+    <definedName name="DNAconc_pooled">Assay!$D$39</definedName>
     <definedName name="endrepair_maxvol">reference!$B$3</definedName>
-    <definedName name="endrepair_targetmass">Assay!$F$17</definedName>
+    <definedName name="endrepair_targetmass">Assay!$F$16</definedName>
     <definedName name="exp_date">Assay!$C$2</definedName>
     <definedName name="exp_id">Assay!$C$5</definedName>
-    <definedName name="exp_notes">Assay!$C$13</definedName>
-    <definedName name="exp_rxns">Assay!$C$12</definedName>
+    <definedName name="exp_notes">Assay!$C$12</definedName>
+    <definedName name="exp_rxns">Assay!$C$11</definedName>
     <definedName name="exp_summary">Assay!$C$9</definedName>
     <definedName name="exp_type">reference!$B$10</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
     <definedName name="exp_version">reference!$B$11</definedName>
-    <definedName name="flowcell_checkpores">Assay!$C$73</definedName>
-    <definedName name="flowcell_chemisty">Assay!$C$72</definedName>
-    <definedName name="flowcell_id">Assay!$C$69</definedName>
+    <definedName name="flowcell_checkpores">Assay!$C$72</definedName>
+    <definedName name="flowcell_chemisty">Assay!$C$71</definedName>
+    <definedName name="flowcell_id">Assay!$C$68</definedName>
     <definedName name="flowcell_maxvol">reference!$B$5</definedName>
-    <definedName name="flowcell_runduration">Assay!$C$74</definedName>
-    <definedName name="flowcell_status">Assay!$C$70</definedName>
-    <definedName name="flowcell_targetmass">Assay!$B$60</definedName>
-    <definedName name="flowcell_usage_hrs">Assay!$C$71</definedName>
-    <definedName name="library_washbuffer">Assay!$P$45</definedName>
+    <definedName name="flowcell_runduration">Assay!$C$73</definedName>
+    <definedName name="flowcell_status">Assay!$C$69</definedName>
+    <definedName name="flowcell_targetmass">Assay!$B$59</definedName>
+    <definedName name="flowcell_usage_hrs">Assay!$C$70</definedName>
+    <definedName name="library_washbuffer">Assay!$P$44</definedName>
     <definedName name="missing_qc_resolution">reference!$B$7</definedName>
-    <definedName name="seq_platform">Assay!$C$68</definedName>
+    <definedName name="seq_platform">Assay!$C$67</definedName>
     <definedName name="vol_calc">reference!$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="445">
   <si>
     <t>Date:</t>
   </si>
@@ -1602,15 +1602,6 @@
     <t>1 per column (avg)</t>
   </si>
   <si>
-    <t>Logic to deal with samples that have not been quantified</t>
-  </si>
-  <si>
-    <t>DNA source:</t>
-  </si>
-  <si>
-    <t>Incorporation of Anophelese protocol</t>
-  </si>
-  <si>
     <t>Sample vol (µl)</t>
   </si>
   <si>
@@ -1745,13 +1736,16 @@
     <t>Sample Type</t>
   </si>
   <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>positive_control</t>
-  </si>
-  <si>
-    <t>negative_control</t>
+    <t>Added sample type</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -1926,7 +1920,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2020,12 +2014,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2338,7 +2326,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2611,7 +2599,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -2630,18 +2618,124 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2656,115 +2750,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2777,7 +2762,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2789,9 +2773,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="47">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2916,41 +2897,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="0" hidden="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <protection locked="1" hidden="0"/>
@@ -3386,6 +3333,43 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -3525,70 +3509,70 @@
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="44"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Extraction ID" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{D655D6C8-1850-4AC0-8484-17625A62737D}" name="Sample Type" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sWGA Identifier" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PCR Identifier" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PCR Dilution Factor" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Extraction ID" dataDxfId="42"/>
+    <tableColumn id="27" xr3:uid="{D655D6C8-1850-4AC0-8484-17625A62737D}" name="Sample Type" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sWGA Identifier" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PCR Identifier" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PCR Dilution Factor" dataDxfId="37"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="38"/>
-    <tableColumn id="26" xr3:uid="{F1EFF32A-7BE1-415D-A6C1-EB6298E86B67}" name="entry" dataDxfId="37">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="36"/>
+    <tableColumn id="26" xr3:uid="{F1EFF32A-7BE1-415D-A6C1-EB6298E86B67}" name="entry" dataDxfId="35">
       <calculatedColumnFormula>IF(OR(ISBLANK(tbl_SeqLib[[#This Row],[Sample ID]]),ISBLANK(endrepair_targetmass)),0,IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,1,2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{001B4B8A-7DCB-4BB4-B720-5DA9C2A7387A}" name="Exact" dataDxfId="36">
+    <tableColumn id="14" xr3:uid="{001B4B8A-7DCB-4BB4-B720-5DA9C2A7387A}" name="Exact" dataDxfId="34">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]&lt;2,"",IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{93494231-5E3B-4D67-8106-A21E3E62E444}" name="Min for col" dataDxfId="35">
+    <tableColumn id="19" xr3:uid="{93494231-5E3B-4D67-8106-A21E3E62E444}" name="Min for col" dataDxfId="33">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDUP(_xlfn.MINIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{1FEA1346-E871-470E-AA2A-C8AFB0F9A249}" name="Max for col" dataDxfId="34">
+    <tableColumn id="20" xr3:uid="{1FEA1346-E871-470E-AA2A-C8AFB0F9A249}" name="Max for col" dataDxfId="32">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDDOWN(_xlfn.MAXIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{6A9EBE31-586B-4F64-B082-46847B0D6428}" name="Avg for col" dataDxfId="33">
+    <tableColumn id="21" xr3:uid="{6A9EBE31-586B-4F64-B082-46847B0D6428}" name="Avg for col" dataDxfId="31">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDUP(AVERAGEIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{D59FA2D5-564A-45ED-A2E9-851026B8F744}" name="3 per col" dataDxfId="32">
+    <tableColumn id="25" xr3:uid="{D59FA2D5-564A-45ED-A2E9-851026B8F744}" name="3 per col" dataDxfId="30">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Min for col]:[Avg for col]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Min for col]:[Avg for col]],"",1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{BAABBDBE-05B7-486D-848A-EDB46E768A26}" name="2 per col" dataDxfId="31">
+    <tableColumn id="17" xr3:uid="{BAABBDBE-05B7-486D-848A-EDB46E768A26}" name="2 per col" dataDxfId="29">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Max for col]:[Avg for col]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Max for col]:[Avg for col]],"",1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FEDA3D60-A493-4564-992B-620C2DCBD54F}" name="1 per col (max)" dataDxfId="30">
+    <tableColumn id="18" xr3:uid="{FEDA3D60-A493-4564-992B-620C2DCBD54F}" name="1 per col (max)" dataDxfId="28">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Max for col]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{B52F91B1-8FA3-4813-9699-EE87E0A73E1F}" name="1 per col (avg)" dataDxfId="29">
+    <tableColumn id="34" xr3:uid="{B52F91B1-8FA3-4813-9699-EE87E0A73E1F}" name="1 per col (avg)" dataDxfId="27">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Avg for col]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{3DBE046E-BBA1-40FE-9D15-A56B3030C6C7}" name="Avg per plate" dataDxfId="28">
+    <tableColumn id="22" xr3:uid="{3DBE046E-BBA1-40FE-9D15-A56B3030C6C7}" name="Avg per plate" dataDxfId="26">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,AVERAGE(tbl_SeqLib[Exact]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{C00DCD81-1FEF-4ABB-8CC7-499C0C2570E9}" name="Max per plate" dataDxfId="27">
+    <tableColumn id="23" xr3:uid="{C00DCD81-1FEF-4ABB-8CC7-499C0C2570E9}" name="Max per plate" dataDxfId="25">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,MAX(tbl_SeqLib[Exact]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{5078A409-FC75-4147-9A85-9D0F799A65C0}" name="2 per plate" dataDxfId="26">
+    <tableColumn id="24" xr3:uid="{5078A409-FC75-4147-9A85-9D0F799A65C0}" name="2 per plate" dataDxfId="24">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Avg per plate]:[Max per plate]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Avg per plate]:[Max per plate]],,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{B05461DD-A312-4983-ABE1-1FB7EFDBEC61}" name="Quantified" dataDxfId="25">
+    <tableColumn id="32" xr3:uid="{B05461DD-A312-4983-ABE1-1FB7EFDBEC61}" name="Quantified" dataDxfId="23">
       <calculatedColumnFormula>IF(vol_calc=reference!$E$23,tbl_SeqLib[[#This Row],[Exact]],IF(vol_calc=reference!$E$24,tbl_SeqLib[[#This Row],[1 per col (max)]],IF(vol_calc=reference!$E$25,tbl_SeqLib[[#This Row],[1 per col (avg)]],IF(vol_calc=reference!$E$26,tbl_SeqLib[[#This Row],[2 per col]],IF(vol_calc=reference!$E$27,tbl_SeqLib[[#This Row],[3 per col]],IF(vol_calc=reference!$E$28,tbl_SeqLib[[#This Row],[Max per plate]],IF(vol_calc=reference!$E$29,tbl_SeqLib[[#This Row],[Avg per plate]],IF(vol_calc=reference!$E$30,tbl_SeqLib[[#This Row],[2 per plate]],"ERROR"))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{31A406DE-6554-495B-953B-40F9644FB053}" name="Avg per plate (missing)" dataDxfId="24">
+    <tableColumn id="30" xr3:uid="{31A406DE-6554-495B-953B-40F9644FB053}" name="Avg per plate (missing)" dataDxfId="22">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=1,ROUNDUP(AVERAGE(tbl_SeqLib[Exact]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{C102ACE7-217E-4DB5-BABC-91C1DAD8AB2B}" name="Avg per col (missing)" dataDxfId="23">
+    <tableColumn id="29" xr3:uid="{C102ACE7-217E-4DB5-BABC-91C1DAD8AB2B}" name="Avg per col (missing)" dataDxfId="21">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=1,ROUNDUP(AVERAGEIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{EF7D6D48-AEC3-450E-B0D6-BDE3BF99E719}" name="Not quantified" dataDxfId="22">
+    <tableColumn id="33" xr3:uid="{EF7D6D48-AEC3-450E-B0D6-BDE3BF99E719}" name="Not quantified" dataDxfId="20">
       <calculatedColumnFormula>IF(missing_qc_resolution=reference!$E$34,tbl_SeqLib[[#This Row],[Avg per col (missing)]],tbl_SeqLib[[#This Row],[Avg per plate (missing)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PCR prodct (µl) to add for end-repair (calculated)" dataDxfId="21">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PCR prodct (µl) to add for end-repair (calculated)" dataDxfId="19">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=0,"",IF(tbl_SeqLib[[#This Row],[entry]]=1,tbl_SeqLib[[#This Row],[Not quantified]],IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Quantified]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{22CC5A4D-2B43-425F-9880-9E27A697A4AC}" name="PCR prodct (µl) added (if different from calculated)" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NF H20 (µl)" dataDxfId="19">
+    <tableColumn id="15" xr3:uid="{22CC5A4D-2B43-425F-9880-9E27A697A4AC}" name="PCR prodct (µl) added (if different from calculated)" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NF H20 (µl)" dataDxfId="17">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=0,"",SUM(endrepair_maxvol-IF(tbl_SeqLib[[#This Row],[PCR prodct (µl) added (if different from calculated)]]&gt;0,tbl_SeqLib[[#This Row],[PCR prodct (µl) added (if different from calculated)]],tbl_SeqLib[[#This Row],[PCR prodct (µl) to add for end-repair (calculated)]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SeqLib Identifier" dataDxfId="18">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SeqLib Identifier" dataDxfId="16">
       <calculatedColumnFormula>IF(ISBLANK(tbl_SeqLib[[#This Row],[sWGA Identifier]]),"",CONCATENATE(exp_id,"_",tbl_SeqLib[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3683,7 +3667,7 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="sample_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="extraction_id"/>
-    <tableColumn id="9" xr3:uid="{C321884E-D42D-45E4-BC5D-30F682C7C762}" name="sample_type" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{C321884E-D42D-45E4-BC5D-30F682C7C762}" name="sample_type" dataDxfId="15">
       <calculatedColumnFormula>IF(LEN(Library!F3)=0,"",Library!F3)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="expt_id"/>
@@ -3881,10 +3865,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3893,1037 +3877,986 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="130" t="s">
         <v>395</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="95"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="97" t="s">
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="97"/>
-      <c r="J2" s="98" t="s">
+      <c r="H2" s="114"/>
+      <c r="J2" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="98"/>
+      <c r="K2" s="132"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="95"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="100" t="s">
+      <c r="J3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="100"/>
+      <c r="K3" s="134"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="95"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="101" t="s">
+      <c r="J4" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="101"/>
+      <c r="K4" s="135"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="103" t="str">
+      <c r="B5" s="125"/>
+      <c r="C5" s="110" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="104"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="105" t="str">
+      <c r="B6" s="125"/>
+      <c r="C6" s="127" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="106"/>
-      <c r="C8" s="107"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="109" t="str">
+      <c r="B9" s="121"/>
+      <c r="C9" s="122" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="109"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="109" t="str">
+      <c r="B10" s="121"/>
+      <c r="C10" s="122" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="109"/>
-      <c r="H10" s="109"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
-        <v>423</v>
+        <v>19</v>
       </c>
       <c r="B11" s="95"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="95" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="95"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="110"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="110"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110"/>
-      <c r="K14" s="110"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="6"/>
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="I15" s="124" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="I16" s="111" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A16" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="9" t="str">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="9" t="str">
         <f>CONCATENATE("ng added, max vol = ", endrepair_maxvol, " µl, max 800ng")</f>
         <v>ng added, max vol = 10 µl, max 800ng</v>
       </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D17" s="33">
         <v>0.1</v>
       </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="112" t="s">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="113" t="s">
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="113"/>
-      <c r="F19" s="113" t="str">
+      <c r="E18" s="120"/>
+      <c r="F18" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G19" s="113"/>
-      <c r="I19" s="114" t="s">
+      <c r="G18" s="120"/>
+      <c r="I18" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="114"/>
-      <c r="K19" s="11" t="s">
+      <c r="J18" s="99"/>
+      <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116" t="s">
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="117" t="s">
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="118" t="s">
+      <c r="E19" s="115"/>
+      <c r="F19" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="118"/>
-      <c r="I20" s="119">
+      <c r="G19" s="116"/>
+      <c r="I19" s="108">
         <v>20</v>
       </c>
-      <c r="J20" s="119"/>
+      <c r="J19" s="108"/>
+      <c r="K19" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="103" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="115" t="str">
+        <f>CONCATENATE(endrepair_maxvol, " - x")</f>
+        <v>10 - x</v>
+      </c>
+      <c r="E20" s="115"/>
+      <c r="F20" s="116" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="116"/>
+      <c r="I20" s="108">
+        <v>65</v>
+      </c>
+      <c r="J20" s="108"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="117" t="str">
-        <f>CONCATENATE(endrepair_maxvol, " - x")</f>
-        <v>10 - x</v>
-      </c>
-      <c r="E21" s="117"/>
-      <c r="F21" s="118" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="118"/>
-      <c r="I21" s="119">
-        <v>65</v>
-      </c>
-      <c r="J21" s="119"/>
-      <c r="K21" s="8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116" t="s">
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="120">
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="118">
         <v>1.4</v>
       </c>
-      <c r="E22" s="120"/>
-      <c r="F22" s="118">
-        <f>SUM(D22*exp_rxns*(1+$D$18))</f>
+      <c r="E21" s="118"/>
+      <c r="F21" s="116">
+        <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="118"/>
-      <c r="I22" s="119">
+      <c r="G21" s="116"/>
+      <c r="I21" s="108">
         <v>4</v>
       </c>
-      <c r="J22" s="119"/>
-      <c r="K22" s="3" t="s">
+      <c r="J21" s="108"/>
+      <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="116" t="s">
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="120">
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="118">
         <v>0.6</v>
       </c>
-      <c r="E23" s="120"/>
-      <c r="F23" s="118">
-        <f>SUM(D23*exp_rxns*(1+$D$18))</f>
+      <c r="E22" s="118"/>
+      <c r="F22" s="116">
+        <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G23" s="118"/>
+      <c r="G22" s="116"/>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="D23" s="119">
+        <f>SUM(D21:D22)+endrepair_maxvol</f>
+        <v>12</v>
+      </c>
+      <c r="E23" s="119"/>
+      <c r="F23" s="13" t="str">
+        <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
+        <v>Add 2 µl of MM to each</v>
+      </c>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
-      <c r="D24" s="121">
-        <f>SUM(D22:D23)+endrepair_maxvol</f>
-        <v>12</v>
-      </c>
-      <c r="E24" s="121"/>
-      <c r="F24" s="13" t="str">
-        <f>CONCATENATE("Add ",SUM(D22:D23)," µl of MM to each")</f>
-        <v>Add 2 µl of MM to each</v>
-      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A25" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="2" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D25" s="10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="112" t="s">
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113" t="s">
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="113"/>
-      <c r="F27" s="113" t="str">
+      <c r="E26" s="120"/>
+      <c r="F26" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G27" s="113"/>
-      <c r="I27" s="114" t="s">
+      <c r="G26" s="120"/>
+      <c r="I26" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="114"/>
-      <c r="K27" s="11" t="s">
+      <c r="J26" s="99"/>
+      <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="103" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="115">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="115"/>
+      <c r="F27" s="116" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="116"/>
+      <c r="I27" s="108">
+        <v>20</v>
+      </c>
+      <c r="J27" s="108"/>
+      <c r="K27" s="8">
+        <v>20</v>
+      </c>
+    </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117">
-        <v>0.5</v>
-      </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="118" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="118"/>
-      <c r="I28" s="119">
-        <v>20</v>
-      </c>
-      <c r="J28" s="119"/>
+      <c r="A28" s="103" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="115">
+        <v>6</v>
+      </c>
+      <c r="E28" s="115"/>
+      <c r="F28" s="116">
+        <f>SUM(D28*exp_rxns*(1+$D$25))</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="116"/>
+      <c r="I28" s="108">
+        <v>65</v>
+      </c>
+      <c r="J28" s="108"/>
       <c r="K28" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117">
-        <v>6</v>
-      </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="118">
-        <f>SUM(D29*exp_rxns*(1+$D$26))</f>
+      <c r="A29" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="115">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="115"/>
+      <c r="F29" s="116">
+        <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="118"/>
-      <c r="I29" s="119">
-        <v>65</v>
-      </c>
-      <c r="J29" s="119"/>
-      <c r="K29" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="116" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="I29" s="108">
+        <v>8</v>
+      </c>
+      <c r="J29" s="108"/>
+      <c r="K29" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="D30" s="117">
-        <v>0.2</v>
+        <f>SUM(D27:D29)+D23</f>
+        <v>18.7</v>
       </c>
       <c r="E30" s="117"/>
-      <c r="F30" s="118">
-        <f>SUM(D30*exp_rxns*(1+$D$26))</f>
+      <c r="F30" s="13" t="str">
+        <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
+        <v>Add 6.2 µl of MM to each</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="87" t="s">
+        <v>422</v>
+      </c>
+      <c r="B33" s="87" t="s">
+        <v>423</v>
+      </c>
+      <c r="C33" s="87" t="s">
+        <v>427</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>425</v>
+      </c>
+      <c r="E33" s="87" t="s">
+        <v>426</v>
+      </c>
+      <c r="F33" s="87" t="s">
+        <v>424</v>
+      </c>
+      <c r="G33" s="87" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="90"/>
+      <c r="B34" s="89" t="str">
+        <f>IF(OR(ISBLANK(A34),ISBLANK(exp_rxns)),"",SUM(A34*exp_rxns))</f>
+        <v/>
+      </c>
+      <c r="C34" s="90">
+        <v>0.4</v>
+      </c>
+      <c r="D34" s="89" t="str">
+        <f>IFERROR(SUM(B34*C34),"")</f>
+        <v/>
+      </c>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="71" t="s">
+        <v>432</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="26"/>
+    </row>
+    <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="113" t="s">
+        <v>431</v>
+      </c>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="114"/>
+      <c r="K36" s="114"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="71" t="s">
+        <v>430</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="101" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="101"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <f>SUM(exp_rxns*D30)*0.4</f>
         <v>0</v>
       </c>
-      <c r="G30" s="118"/>
-      <c r="I30" s="119">
-        <v>8</v>
-      </c>
-      <c r="J30" s="119"/>
-      <c r="K30" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="D31" s="122">
-        <f>SUM(D28:D30)+D24</f>
-        <v>18.7</v>
-      </c>
-      <c r="E31" s="122"/>
-      <c r="F31" s="13" t="str">
-        <f>CONCATENATE("Add ",SUM(D29:D30)," µl of MM to each")</f>
-        <v>Add 6.2 µl of MM to each</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="87" t="s">
-        <v>425</v>
-      </c>
-      <c r="B34" s="87" t="s">
-        <v>426</v>
-      </c>
-      <c r="C34" s="87" t="s">
-        <v>430</v>
-      </c>
-      <c r="D34" s="87" t="s">
-        <v>428</v>
-      </c>
-      <c r="E34" s="87" t="s">
-        <v>429</v>
-      </c>
-      <c r="F34" s="87" t="s">
-        <v>427</v>
-      </c>
-      <c r="G34" s="87" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="90"/>
-      <c r="B35" s="89" t="str">
-        <f>IF(OR(ISBLANK(A35),ISBLANK(exp_rxns)),"",SUM(A35*exp_rxns))</f>
-        <v/>
-      </c>
-      <c r="C35" s="90">
-        <v>0.4</v>
-      </c>
-      <c r="D35" s="89" t="str">
-        <f>IFERROR(SUM(B35*C35),"")</f>
-        <v/>
-      </c>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="90"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="71" t="s">
-        <v>435</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="127" t="s">
-        <v>434</v>
-      </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="97"/>
-      <c r="K37" s="97"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71" t="s">
-        <v>433</v>
-      </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="123" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="123"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
-        <f>SUM(exp_rxns*D31)*0.4</f>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="112">
+        <f>SUM(B39*C39)</f>
         <v>0</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="124">
-        <f>SUM(B40*C40)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="124"/>
+      <c r="E39" s="112"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A42" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="9" t="s">
+      <c r="B42" s="28"/>
+      <c r="C42" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="F43" s="28">
+      <c r="F42" s="28">
         <v>50</v>
       </c>
-      <c r="G43" s="5" t="str">
+      <c r="G42" s="5" t="str">
         <f>_xlfn.CONCAT("µl (recommend 1500 ng of product in ",adaptlig_dna_maxvol," µl max)")</f>
         <v>µl (recommend 1500 ng of product in 30 µl max)</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="114" t="s">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="125" t="s">
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="125"/>
-      <c r="I44" s="114" t="s">
+      <c r="E43" s="100"/>
+      <c r="I43" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J44" s="114"/>
-      <c r="K44" s="11" t="s">
+      <c r="J43" s="99"/>
+      <c r="K43" s="11" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="102">
+        <f>IF(B39="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D39)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D39)))</f>
+        <v>30</v>
+      </c>
+      <c r="E44" s="102"/>
+      <c r="F44" s="5"/>
+      <c r="I44" s="108" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" s="108"/>
+      <c r="K44" s="8">
+        <v>10</v>
+      </c>
+    </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="126">
-        <f>IF(B40="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D40)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D40)))</f>
-        <v>30</v>
-      </c>
-      <c r="E45" s="126"/>
-      <c r="F45" s="5"/>
-      <c r="I45" s="119" t="s">
-        <v>47</v>
-      </c>
-      <c r="J45" s="119"/>
-      <c r="K45" s="8">
-        <v>10</v>
-      </c>
+      <c r="A45" s="103" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="103"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="102">
+        <f>IFERROR(SUM(adaptlig_dna_maxvol-D44),"")</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="102"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="116" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="126">
-        <f>IFERROR(SUM(adaptlig_dna_maxvol-D45),"")</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="126"/>
-      <c r="F46" s="8"/>
+      <c r="A46" s="103" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="103"/>
+      <c r="C46" s="103"/>
+      <c r="D46" s="110">
+        <v>5</v>
+      </c>
+      <c r="E46" s="110"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="116" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="103">
-        <v>5</v>
-      </c>
-      <c r="E47" s="103"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="116" t="s">
+      <c r="A47" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="103">
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="110">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E48" s="103"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="116" t="s">
+      <c r="E47" s="110"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="103">
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="110">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E49" s="103"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D50" s="128">
-        <f>SUM(D45:D49)</f>
+      <c r="E48" s="110"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D49" s="111">
+        <f>SUM(D44:D48)</f>
         <v>50</v>
       </c>
-      <c r="E50" s="128"/>
+      <c r="E49" s="111"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>389</v>
+      <c r="B52" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="71" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C53" s="47"/>
-      <c r="D53" s="71" t="s">
-        <v>432</v>
-      </c>
+      <c r="A53" s="109" t="s">
+        <v>391</v>
+      </c>
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="131" t="s">
-        <v>391</v>
-      </c>
-      <c r="B54" s="131"/>
-      <c r="C54" s="131"/>
-      <c r="D54" s="131"/>
-      <c r="E54" s="131"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="131"/>
-      <c r="I54" s="131"/>
-      <c r="J54" s="131"/>
-      <c r="K54" s="131"/>
-      <c r="L54" s="131"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="71" t="s">
-        <v>433</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="I55" s="71"/>
-      <c r="J55" s="71"/>
-      <c r="K55" s="71"/>
-      <c r="L55" s="88"/>
-    </row>
-    <row r="56" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="112" t="s">
+      <c r="A54" s="71" t="s">
+        <v>430</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="I54" s="71"/>
+      <c r="J54" s="71"/>
+      <c r="K54" s="71"/>
+      <c r="L54" s="88"/>
+    </row>
+    <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="112"/>
-      <c r="C56" s="112" t="s">
+      <c r="B55" s="105"/>
+      <c r="C55" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112" t="s">
+      <c r="D55" s="105"/>
+      <c r="E55" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112" t="s">
+      <c r="F55" s="105"/>
+      <c r="G55" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="H56" s="112"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="129">
+      <c r="H55" s="105"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="106">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B57" s="129"/>
-      <c r="C57" s="130"/>
-      <c r="D57" s="130"/>
-      <c r="E57" s="130"/>
-      <c r="F57" s="130"/>
-      <c r="G57" s="119">
-        <f>SUM(C57*E57)</f>
+      <c r="B56" s="106"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="108">
+        <f>SUM(C56*E56)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="119"/>
+      <c r="H56" s="108"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="A59" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="9" t="str">
+      <c r="B59" s="28"/>
+      <c r="C59" s="9" t="str">
         <f>CONCATENATE("ng of library (max volume = ", flowcell_maxvol,"µl), recommend 800 ng")</f>
         <v>ng of library (max volume = 12µl), recommend 800 ng</v>
       </c>
-      <c r="H60" s="18"/>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="99"/>
+      <c r="C60" s="99"/>
+      <c r="D60" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="100"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="114" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="114"/>
-      <c r="C61" s="114"/>
-      <c r="D61" s="125" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" s="125"/>
+      <c r="A61" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="101"/>
+      <c r="C61" s="101"/>
+      <c r="D61" s="102">
+        <f>IF(C56="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G56)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G56)))</f>
+        <v>12</v>
+      </c>
+      <c r="E61" s="102"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="123" t="s">
-        <v>53</v>
-      </c>
-      <c r="B62" s="123"/>
-      <c r="C62" s="123"/>
-      <c r="D62" s="126">
-        <f>IF(C57="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G57)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G57)))</f>
-        <v>12</v>
-      </c>
-      <c r="E62" s="126"/>
+      <c r="A62" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="101"/>
+      <c r="C62" s="101"/>
+      <c r="D62" s="102" t="str">
+        <f>IFERROR((IF(SUM(12-D61)=0,"-",SUM(12-D61))),"")</f>
+        <v>-</v>
+      </c>
+      <c r="E62" s="102"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="123" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" s="123"/>
-      <c r="C63" s="123"/>
-      <c r="D63" s="126" t="str">
-        <f>IFERROR((IF(SUM(12-D62)=0,"-",SUM(12-D62))),"")</f>
-        <v>-</v>
-      </c>
-      <c r="E63" s="126"/>
+      <c r="A63" s="103" t="s">
+        <v>396</v>
+      </c>
+      <c r="B63" s="103"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="104">
+        <v>37.5</v>
+      </c>
+      <c r="E63" s="104"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="116" t="s">
-        <v>396</v>
-      </c>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="132">
-        <v>37.5</v>
-      </c>
-      <c r="E64" s="132"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="116" t="s">
+      <c r="A64" s="103" t="s">
         <v>397</v>
       </c>
-      <c r="B65" s="116"/>
-      <c r="C65" s="116"/>
-      <c r="D65" s="132">
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="104">
         <v>25.5</v>
       </c>
-      <c r="E65" s="132"/>
-      <c r="F65" s="5" t="s">
+      <c r="E64" s="104"/>
+      <c r="F64" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="5"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="95"/>
+      <c r="C67" s="97"/>
+      <c r="D67" s="97"/>
+      <c r="E67" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="95" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B68" s="95"/>
-      <c r="C68" s="134"/>
-      <c r="D68" s="134"/>
-      <c r="E68" s="5" t="s">
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="95"/>
+      <c r="C69" s="96"/>
+      <c r="D69" s="96"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="95" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="95"/>
+      <c r="C70" s="98" t="str">
+        <f>IF(flowcell_status="New",0,"")</f>
+        <v/>
+      </c>
+      <c r="D70" s="98"/>
+      <c r="E70" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="95" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="95"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="97"/>
+      <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="133"/>
-      <c r="D69" s="133"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" s="95"/>
-      <c r="C70" s="133"/>
-      <c r="D70" s="133"/>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="95" t="s">
-        <v>61</v>
-      </c>
-      <c r="B71" s="95"/>
-      <c r="C71" s="135" t="str">
-        <f>IF(flowcell_status="New",0,"")</f>
-        <v/>
-      </c>
-      <c r="D71" s="135"/>
-      <c r="E71" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="95" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B72" s="95"/>
-      <c r="C72" s="134"/>
-      <c r="D72" s="134"/>
-      <c r="E72" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="95" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B73" s="95"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="133"/>
+      <c r="C73" s="96"/>
+      <c r="D73" s="96"/>
       <c r="E73" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="95" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="95"/>
-      <c r="C74" s="133"/>
-      <c r="D74" s="133"/>
-      <c r="E74" s="9" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="118">
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="A54:L54"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
+  <mergeCells count="116">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
@@ -4935,98 +4868,132 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:K14"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
   </mergeCells>
-  <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="15" priority="5">
-      <formula>COUNTIF(A35,"")</formula>
+  <conditionalFormatting sqref="A34 C11:C12">
+    <cfRule type="expression" dxfId="14" priority="5">
+      <formula>COUNTIF(A11,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B60">
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula>COUNTIF(B60,"")</formula>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>COUNTIF(B59,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C4 C7:C8 C11:C13 F17 B40:C40 B43 C57:E57 C68:C70 C72:C74">
-    <cfRule type="expression" dxfId="13" priority="10">
+  <conditionalFormatting sqref="C2:C4 C7:C8 F16 B39:C39 B42 C56:E56 C67:C69 C71:C73">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>COUNTIF(B2,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>COUNTIF(C35,"")</formula>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>COUNTIF(C34,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="11" priority="2">
-      <formula>COUNTIF(C53,"")</formula>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>COUNTIF(C52,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
+  <conditionalFormatting sqref="C72">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThan">
       <formula>800</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="greaterThanOrEqual">
       <formula>800</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="lessThan">
+  <conditionalFormatting sqref="D39">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:G35">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>COUNTIF(E35,"")</formula>
+  <conditionalFormatting sqref="E34:G34">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>COUNTIF(E34,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>COUNTIF(F43,"")</formula>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>COUNTIF(F42,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G57">
-    <cfRule type="cellIs" dxfId="3" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="G56">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5035,11 +5002,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum 200ng / Maximum 800 ng should be added per sample" sqref="F17" xr:uid="{77FA29BE-4BF7-4DBB-8F9D-E8DA28B60EE6}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Minimum 200ng / Maximum 800 ng should be added per sample" sqref="F16" xr:uid="{77FA29BE-4BF7-4DBB-8F9D-E8DA28B60EE6}">
       <formula1>200</formula1>
       <formula2>800</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60" xr:uid="{9692DBAD-DA3C-491D-943D-13D26695D34C}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{9692DBAD-DA3C-491D-943D-13D26695D34C}">
       <formula1>400</formula1>
       <formula2>1500</formula2>
     </dataValidation>
@@ -5054,7 +5021,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="17" id="{7D748971-4ED9-4DAD-A430-377FADB0435A}">
-            <xm:f>COUNTIF($C$70,reference!$E$4)</xm:f>
+            <xm:f>COUNTIF($C$69,reference!$E$4)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -5063,7 +5030,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C71</xm:sqref>
+          <xm:sqref>C70</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5076,25 +5043,25 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C70</xm:sqref>
+          <xm:sqref>C69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9EA06E1-B72E-4158-9E78-547DCB9CC597}">
           <x14:formula1>
             <xm:f>reference!$E$7:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F43</xm:sqref>
+          <xm:sqref>F42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86E97738-BE4E-45D2-82E4-9BB20B6C5270}">
           <x14:formula1>
             <xm:f>reference!$E$11:$E$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C68:D68</xm:sqref>
+          <xm:sqref>C67:D67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FD70BE5-C9FE-4FC2-BCF1-8C135E992CE5}">
           <x14:formula1>
             <xm:f>reference!$E$18:$E$19</xm:f>
           </x14:formula1>
-          <xm:sqref>C72:D72</xm:sqref>
+          <xm:sqref>C71:D71</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -5118,13 +5085,13 @@
           <x14:formula1>
             <xm:f>reference!$E$38:$E$39</xm:f>
           </x14:formula1>
-          <xm:sqref>F35</xm:sqref>
+          <xm:sqref>F34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8AB4769-634A-4E55-85CA-F2BAE73B69BB}">
           <x14:formula1>
             <xm:f>reference!$E$42:$E$43</xm:f>
           </x14:formula1>
-          <xm:sqref>G35</xm:sqref>
+          <xm:sqref>G34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5212,7 +5179,7 @@
         <v>76</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G2" s="74" t="s">
         <v>77</v>
@@ -15307,8 +15274,8 @@
     <mergeCell ref="L1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="L3:L98 D1:J98">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="D1:J98 L3:L98">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>COUNTIF(D1,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15544,7 +15511,7 @@
         <v>305</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>58</v>
@@ -15578,7 +15545,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="E14" t="s">
         <v>359</v>
@@ -15588,9 +15555,6 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>424</v>
-      </c>
       <c r="E15" s="15" t="s">
         <v>360</v>
       </c>
@@ -15726,10 +15690,10 @@
     </row>
     <row r="37" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E37" s="83" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F37" s="80" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.25">
@@ -15737,7 +15701,7 @@
         <v>700</v>
       </c>
       <c r="F38" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.25">
@@ -15745,15 +15709,15 @@
         <v>200</v>
       </c>
       <c r="F39" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="41" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E41" s="83" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.25">
@@ -15761,7 +15725,7 @@
         <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="5:6" x14ac:dyDescent="0.25">
@@ -15769,27 +15733,27 @@
         <v>70</v>
       </c>
       <c r="F43" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="45" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="139" t="s">
-        <v>443</v>
+      <c r="E45" s="94" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="46" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="47" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="48" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -16193,7 +16157,7 @@
       </c>
       <c r="E2">
         <f>IF(LEN(exp_version)=0,"",exp_version)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" t="str">
         <f>IF(LEN(exp_notes)=0,"",exp_notes)</f>
@@ -16311,7 +16275,7 @@
         <v>330</v>
       </c>
       <c r="C1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D1" t="s">
         <v>306</v>

</xml_diff>

<commit_message>
Updated templates to better handle various enzyme and panel combinations, plus better error checking
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64991F3C-DFA7-403A-8196-42FD23760DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5920D7-6B42-4FEA-BC1F-789DC200E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29625" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -2619,37 +2619,103 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2664,91 +2730,25 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -3867,8 +3867,8 @@
   </sheetPr>
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3877,171 +3877,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="130" t="s">
         <v>395</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="98" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="J2" s="99" t="s">
+      <c r="H2" s="114"/>
+      <c r="J2" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="99"/>
+      <c r="K2" s="132"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="101"/>
+      <c r="K3" s="134"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="102" t="s">
+      <c r="J4" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="102"/>
+      <c r="K4" s="135"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="104" t="str">
+      <c r="B5" s="125"/>
+      <c r="C5" s="110" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="105" t="s">
+      <c r="J5" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="105"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="103"/>
-      <c r="C6" s="106" t="str">
+      <c r="B6" s="125"/>
+      <c r="C6" s="127" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="107"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="109"/>
-      <c r="C9" s="110" t="str">
+      <c r="B9" s="121"/>
+      <c r="C9" s="122" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="109"/>
-      <c r="C10" s="110" t="str">
+      <c r="B10" s="121"/>
+      <c r="C10" s="122" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="96"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="27"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -4049,32 +4049,32 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
@@ -4085,11 +4085,11 @@
       </c>
       <c r="C15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="112" t="s">
+      <c r="I15" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -4119,119 +4119,119 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="113" t="s">
+      <c r="A18" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="114" t="s">
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114" t="str">
+      <c r="E18" s="120"/>
+      <c r="F18" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="I18" s="115" t="s">
+      <c r="G18" s="120"/>
+      <c r="I18" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="115"/>
+      <c r="J18" s="99"/>
       <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="117" t="s">
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="117"/>
-      <c r="F19" s="118" t="s">
+      <c r="E19" s="115"/>
+      <c r="F19" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="118"/>
-      <c r="I19" s="119">
+      <c r="G19" s="116"/>
+      <c r="I19" s="108">
         <v>20</v>
       </c>
-      <c r="J19" s="119"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="117" t="str">
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="115" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="118" t="s">
+      <c r="E20" s="115"/>
+      <c r="F20" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="118"/>
-      <c r="I20" s="119">
+      <c r="G20" s="116"/>
+      <c r="I20" s="108">
         <v>65</v>
       </c>
-      <c r="J20" s="119"/>
+      <c r="J20" s="108"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="120">
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="118">
         <v>1.4</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="118">
+      <c r="E21" s="118"/>
+      <c r="F21" s="116">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="118"/>
-      <c r="I21" s="119">
+      <c r="G21" s="116"/>
+      <c r="I21" s="108">
         <v>4</v>
       </c>
-      <c r="J21" s="119"/>
+      <c r="J21" s="108"/>
       <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="120">
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="118">
         <v>0.6</v>
       </c>
-      <c r="E22" s="120"/>
-      <c r="F22" s="118">
+      <c r="E22" s="118"/>
+      <c r="F22" s="116">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="118"/>
+      <c r="G22" s="116"/>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="D23" s="121">
+      <c r="D23" s="119">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="121"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -4256,103 +4256,103 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="114" t="s">
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114" t="str">
+      <c r="E26" s="120"/>
+      <c r="F26" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="114"/>
-      <c r="I26" s="115" t="s">
+      <c r="G26" s="120"/>
+      <c r="I26" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="115"/>
+      <c r="J26" s="99"/>
       <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117">
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="115">
         <v>0.5</v>
       </c>
-      <c r="E27" s="117"/>
-      <c r="F27" s="118" t="s">
+      <c r="E27" s="115"/>
+      <c r="F27" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="118"/>
-      <c r="I27" s="119">
+      <c r="G27" s="116"/>
+      <c r="I27" s="108">
         <v>20</v>
       </c>
-      <c r="J27" s="119"/>
+      <c r="J27" s="108"/>
       <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117">
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="115">
         <v>6</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="118">
+      <c r="E28" s="115"/>
+      <c r="F28" s="116">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="118"/>
-      <c r="I28" s="119">
+      <c r="G28" s="116"/>
+      <c r="I28" s="108">
         <v>65</v>
       </c>
-      <c r="J28" s="119"/>
+      <c r="J28" s="108"/>
       <c r="K28" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117">
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="115">
         <v>0.2</v>
       </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="118">
+      <c r="E29" s="115"/>
+      <c r="F29" s="116">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="118"/>
-      <c r="I29" s="119">
+      <c r="G29" s="116"/>
+      <c r="I29" s="108">
         <v>8</v>
       </c>
-      <c r="J29" s="119"/>
+      <c r="J29" s="108"/>
       <c r="K29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="D30" s="122">
+      <c r="D30" s="117">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="122"/>
+      <c r="E30" s="117"/>
       <c r="F30" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -4416,19 +4416,19 @@
       <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="113" t="s">
         <v>431</v>
       </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="114"/>
+      <c r="K36" s="114"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="71" t="s">
@@ -4451,10 +4451,10 @@
       <c r="C38" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="123" t="s">
+      <c r="D38" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="123"/>
+      <c r="E38" s="101"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
-      <c r="D39" s="124">
+      <c r="D39" s="112">
         <f>SUM(B39*C39)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="124"/>
+      <c r="E39" s="112"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4491,97 +4491,97 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="115" t="s">
+      <c r="A43" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="115"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="125" t="s">
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="125"/>
-      <c r="I43" s="115" t="s">
+      <c r="E43" s="100"/>
+      <c r="I43" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="115"/>
+      <c r="J43" s="99"/>
       <c r="K43" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="116"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="126">
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="102">
         <f>IF(B39="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D39)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D39)))</f>
         <v>30</v>
       </c>
-      <c r="E44" s="126"/>
+      <c r="E44" s="102"/>
       <c r="F44" s="5"/>
-      <c r="I44" s="119" t="s">
+      <c r="I44" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="119"/>
+      <c r="J44" s="108"/>
       <c r="K44" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="126">
+      <c r="B45" s="103"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="102">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D44),"")</f>
         <v>0</v>
       </c>
-      <c r="E45" s="126"/>
+      <c r="E45" s="102"/>
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="116" t="s">
+      <c r="A46" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="104">
+      <c r="B46" s="103"/>
+      <c r="C46" s="103"/>
+      <c r="D46" s="110">
         <v>5</v>
       </c>
-      <c r="E46" s="104"/>
+      <c r="E46" s="110"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="116" t="s">
+      <c r="A47" s="103" t="s">
         <v>388</v>
       </c>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="104">
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="110">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E47" s="104"/>
+      <c r="E47" s="110"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="104">
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="110">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E48" s="104"/>
+      <c r="E48" s="110"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="128">
+      <c r="D49" s="111">
         <f>SUM(D44:D48)</f>
         <v>50</v>
       </c>
-      <c r="E49" s="128"/>
+      <c r="E49" s="111"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
@@ -4598,20 +4598,20 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="131" t="s">
+      <c r="A53" s="109" t="s">
         <v>391</v>
       </c>
-      <c r="B53" s="131"/>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="131"/>
-      <c r="H53" s="131"/>
-      <c r="I53" s="131"/>
-      <c r="J53" s="131"/>
-      <c r="K53" s="131"/>
-      <c r="L53" s="131"/>
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="71" t="s">
@@ -4629,38 +4629,38 @@
       <c r="L54" s="88"/>
     </row>
     <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="113" t="s">
+      <c r="A55" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="113"/>
-      <c r="C55" s="113" t="s">
+      <c r="B55" s="105"/>
+      <c r="C55" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="113"/>
-      <c r="E55" s="113" t="s">
+      <c r="D55" s="105"/>
+      <c r="E55" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="F55" s="113"/>
-      <c r="G55" s="113" t="s">
+      <c r="F55" s="105"/>
+      <c r="G55" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="113"/>
+      <c r="H55" s="105"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="129">
+      <c r="A56" s="106">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="130"/>
-      <c r="E56" s="130"/>
-      <c r="F56" s="130"/>
-      <c r="G56" s="119">
+      <c r="B56" s="106"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="108">
         <f>SUM(C56*E56)</f>
         <v>0</v>
       </c>
-      <c r="H56" s="119"/>
+      <c r="H56" s="108"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
@@ -4679,61 +4679,61 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="115" t="s">
+      <c r="A60" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="115"/>
-      <c r="C60" s="115"/>
-      <c r="D60" s="125" t="s">
+      <c r="B60" s="99"/>
+      <c r="C60" s="99"/>
+      <c r="D60" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="125"/>
+      <c r="E60" s="100"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="123" t="s">
+      <c r="A61" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="123"/>
-      <c r="C61" s="123"/>
-      <c r="D61" s="126">
+      <c r="B61" s="101"/>
+      <c r="C61" s="101"/>
+      <c r="D61" s="102">
         <f>IF(C56="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G56)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G56)))</f>
         <v>12</v>
       </c>
-      <c r="E61" s="126"/>
+      <c r="E61" s="102"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="123" t="s">
+      <c r="A62" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="123"/>
-      <c r="C62" s="123"/>
-      <c r="D62" s="126" t="str">
+      <c r="B62" s="101"/>
+      <c r="C62" s="101"/>
+      <c r="D62" s="102" t="str">
         <f>IFERROR((IF(SUM(12-D61)=0,"-",SUM(12-D61))),"")</f>
         <v>-</v>
       </c>
-      <c r="E62" s="126"/>
+      <c r="E62" s="102"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="116" t="s">
+      <c r="A63" s="103" t="s">
         <v>396</v>
       </c>
-      <c r="B63" s="116"/>
-      <c r="C63" s="116"/>
-      <c r="D63" s="132">
+      <c r="B63" s="103"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="104">
         <v>37.5</v>
       </c>
-      <c r="E63" s="132"/>
+      <c r="E63" s="104"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="116" t="s">
+      <c r="A64" s="103" t="s">
         <v>397</v>
       </c>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="132">
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="104">
         <v>25.5</v>
       </c>
-      <c r="E64" s="132"/>
+      <c r="E64" s="104"/>
       <c r="F64" s="5" t="s">
         <v>55</v>
       </c>
@@ -4745,75 +4745,75 @@
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="134"/>
-      <c r="D67" s="134"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="97"/>
+      <c r="D67" s="97"/>
       <c r="E67" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="96" t="s">
+      <c r="A68" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="96"/>
-      <c r="C68" s="133"/>
-      <c r="D68" s="133"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="96" t="s">
+      <c r="A69" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="96"/>
-      <c r="C69" s="133"/>
-      <c r="D69" s="133"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="96"/>
+      <c r="D69" s="96"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="135" t="str">
+      <c r="B70" s="95"/>
+      <c r="C70" s="98" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D70" s="135"/>
+      <c r="D70" s="98"/>
       <c r="E70" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="96" t="s">
+      <c r="A71" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="96"/>
-      <c r="C71" s="134"/>
-      <c r="D71" s="134"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="97"/>
       <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="96" t="s">
+      <c r="A72" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="96"/>
-      <c r="C72" s="133"/>
-      <c r="D72" s="133"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
       <c r="E72" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="96"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="133"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="96"/>
+      <c r="D73" s="96"/>
       <c r="E73" s="9" t="s">
         <v>68</v>
       </c>
@@ -4821,6 +4821,108 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="116">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="A73:B73"/>
@@ -4835,108 +4937,6 @@
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="C71:D71"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B59">
     <cfRule type="expression" dxfId="14" priority="7">
@@ -4997,7 +4997,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." sqref="C9:F9 C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -5009,6 +5009,9 @@
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59" xr:uid="{9692DBAD-DA3C-491D-943D-13D26695D34C}">
       <formula1>400</formula1>
       <formula2>1500</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Format" error="Exp Number should be three digits long" sqref="C4:F4" xr:uid="{FE99E680-8F58-4329-B56C-E890C7BD5615}">
+      <formula1>LEN(C4)=3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74861111111111101" header="0.511811023622047" footer="0.31527777777777799"/>

</xml_diff>

<commit_message>
Added function to generate templates for each group to remove need for  manual names/projects entry
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5920D7-6B42-4FEA-BC1F-789DC200E342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1D759C-D272-47AA-BDC8-1B72C3D31CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="23280" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -1479,15 +1479,6 @@
     <t>PC</t>
   </si>
   <si>
-    <t>Project 1</t>
-  </si>
-  <si>
-    <t>Project 2</t>
-  </si>
-  <si>
-    <t>Project 3</t>
-  </si>
-  <si>
     <t>Ligation Buffer (LIS)</t>
   </si>
   <si>
@@ -1746,6 +1737,15 @@
   </si>
   <si>
     <t>Negative</t>
+  </si>
+  <si>
+    <t>Project A</t>
+  </si>
+  <si>
+    <t>Project B</t>
+  </si>
+  <si>
+    <t>Project C</t>
   </si>
 </sst>
 </file>
@@ -2619,87 +2619,50 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2714,41 +2677,78 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -3868,230 +3868,230 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="8" width="9" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="114" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="114"/>
-      <c r="J2" s="132" t="s">
+      <c r="H2" s="98"/>
+      <c r="J2" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="132"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="95" t="s">
+      <c r="K2" s="99"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="134" t="s">
+      <c r="J3" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="134"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95" t="s">
+      <c r="K3" s="101"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="135" t="s">
+      <c r="J4" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="135"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="125" t="s">
+      <c r="K4" s="102"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="125"/>
-      <c r="C5" s="110" t="str">
-        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
-        <v/>
-      </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="104" t="str">
+        <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!I3:J9,2,FALSE()),C4))</f>
+        <v/>
+      </c>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="126" t="s">
+      <c r="J5" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="126"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="125" t="s">
+      <c r="K5" s="105"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="125"/>
-      <c r="C6" s="127" t="str">
+      <c r="B6" s="103"/>
+      <c r="C6" s="106" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="106"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128" t="s">
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="128"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128" t="s">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="128"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="121" t="s">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="121"/>
-      <c r="C9" s="122" t="str">
+      <c r="B9" s="109"/>
+      <c r="C9" s="110" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121" t="s">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="121"/>
-      <c r="C10" s="122" t="str">
+      <c r="B10" s="109"/>
+      <c r="C10" s="110" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="95"/>
+      <c r="B11" s="96"/>
       <c r="C11" s="27"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="95" t="s">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="95"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="96"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="124" t="s">
+      <c r="I15" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>337</v>
       </c>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -4118,132 +4118,132 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="105" t="s">
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="105"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="120" t="s">
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="120"/>
-      <c r="F18" s="120" t="str">
+      <c r="E18" s="114"/>
+      <c r="F18" s="114" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="120"/>
-      <c r="I18" s="99" t="s">
+      <c r="G18" s="114"/>
+      <c r="I18" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="99"/>
+      <c r="J18" s="115"/>
       <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="103"/>
-      <c r="C19" s="103"/>
-      <c r="D19" s="115" t="s">
+      <c r="B19" s="116"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="115"/>
-      <c r="F19" s="116" t="s">
+      <c r="E19" s="117"/>
+      <c r="F19" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="116"/>
-      <c r="I19" s="108">
+      <c r="G19" s="118"/>
+      <c r="I19" s="119">
         <v>20</v>
       </c>
-      <c r="J19" s="108"/>
+      <c r="J19" s="119"/>
       <c r="K19" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="103"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="115" t="str">
+      <c r="B20" s="116"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="117" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="115"/>
-      <c r="F20" s="116" t="s">
+      <c r="E20" s="117"/>
+      <c r="F20" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="116"/>
-      <c r="I20" s="108">
+      <c r="G20" s="118"/>
+      <c r="I20" s="119">
         <v>65</v>
       </c>
-      <c r="J20" s="108"/>
+      <c r="J20" s="119"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="103" t="s">
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="118">
+      <c r="B21" s="116"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="120">
         <v>1.4</v>
       </c>
-      <c r="E21" s="118"/>
-      <c r="F21" s="116">
+      <c r="E21" s="120"/>
+      <c r="F21" s="118">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="116"/>
-      <c r="I21" s="108">
+      <c r="G21" s="118"/>
+      <c r="I21" s="119">
         <v>4</v>
       </c>
-      <c r="J21" s="108"/>
+      <c r="J21" s="119"/>
       <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="103" t="s">
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="118">
+      <c r="B22" s="116"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="120">
         <v>0.6</v>
       </c>
-      <c r="E22" s="118"/>
-      <c r="F22" s="116">
+      <c r="E22" s="120"/>
+      <c r="F22" s="118">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="116"/>
-    </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="118"/>
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
-      <c r="D23" s="119">
+      <c r="D23" s="121">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="119"/>
+      <c r="E23" s="121"/>
       <c r="F23" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>36</v>
       </c>
@@ -4255,139 +4255,139 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="105" t="s">
+    <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="120" t="s">
+      <c r="B26" s="113"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="120"/>
-      <c r="F26" s="120" t="str">
+      <c r="E26" s="114"/>
+      <c r="F26" s="114" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="120"/>
-      <c r="I26" s="99" t="s">
+      <c r="G26" s="114"/>
+      <c r="I26" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="99"/>
+      <c r="J26" s="115"/>
       <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="103" t="s">
+    <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="103"/>
-      <c r="C27" s="103"/>
-      <c r="D27" s="115">
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="117">
         <v>0.5</v>
       </c>
-      <c r="E27" s="115"/>
-      <c r="F27" s="116" t="s">
+      <c r="E27" s="117"/>
+      <c r="F27" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="116"/>
-      <c r="I27" s="108">
+      <c r="G27" s="118"/>
+      <c r="I27" s="119">
         <v>20</v>
       </c>
-      <c r="J27" s="108"/>
+      <c r="J27" s="119"/>
       <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="103" t="s">
+    <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="115">
+      <c r="B28" s="116"/>
+      <c r="C28" s="116"/>
+      <c r="D28" s="117">
         <v>6</v>
       </c>
-      <c r="E28" s="115"/>
-      <c r="F28" s="116">
+      <c r="E28" s="117"/>
+      <c r="F28" s="118">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="116"/>
-      <c r="I28" s="108">
+      <c r="G28" s="118"/>
+      <c r="I28" s="119">
         <v>65</v>
       </c>
-      <c r="J28" s="108"/>
+      <c r="J28" s="119"/>
       <c r="K28" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="103" t="s">
+    <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="103"/>
-      <c r="D29" s="115">
+      <c r="B29" s="116"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="117">
         <v>0.2</v>
       </c>
-      <c r="E29" s="115"/>
-      <c r="F29" s="116">
+      <c r="E29" s="117"/>
+      <c r="F29" s="118">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="116"/>
-      <c r="I29" s="108">
+      <c r="G29" s="118"/>
+      <c r="I29" s="119">
         <v>8</v>
       </c>
-      <c r="J29" s="108"/>
+      <c r="J29" s="119"/>
       <c r="K29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
-      <c r="D30" s="117">
+      <c r="D30" s="122">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="117"/>
+      <c r="E30" s="122"/>
       <c r="F30" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="8"/>
     </row>
-    <row r="33" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="87" t="s">
+        <v>419</v>
+      </c>
+      <c r="B33" s="87" t="s">
+        <v>420</v>
+      </c>
+      <c r="C33" s="87" t="s">
+        <v>424</v>
+      </c>
+      <c r="D33" s="87" t="s">
         <v>422</v>
       </c>
-      <c r="B33" s="87" t="s">
+      <c r="E33" s="87" t="s">
         <v>423</v>
       </c>
-      <c r="C33" s="87" t="s">
-        <v>427</v>
-      </c>
-      <c r="D33" s="87" t="s">
+      <c r="F33" s="87" t="s">
+        <v>421</v>
+      </c>
+      <c r="G33" s="87" t="s">
         <v>425</v>
       </c>
-      <c r="E33" s="87" t="s">
-        <v>426</v>
-      </c>
-      <c r="F33" s="87" t="s">
-        <v>424</v>
-      </c>
-      <c r="G33" s="87" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="90"/>
       <c r="B34" s="89" t="str">
         <f>IF(OR(ISBLANK(A34),ISBLANK(exp_rxns)),"",SUM(A34*exp_rxns))</f>
@@ -4404,9 +4404,9 @@
       <c r="F34" s="90"/>
       <c r="G34" s="90"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="71" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -4415,24 +4415,24 @@
       <c r="F35" s="9"/>
       <c r="G35" s="26"/>
     </row>
-    <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="113" t="s">
-        <v>431</v>
-      </c>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
-      <c r="E36" s="114"/>
-      <c r="F36" s="114"/>
-      <c r="G36" s="114"/>
-      <c r="H36" s="114"/>
-      <c r="I36" s="114"/>
-      <c r="J36" s="114"/>
-      <c r="K36" s="114"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="127" t="s">
+        <v>428</v>
+      </c>
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="71" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -4441,7 +4441,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>41</v>
       </c>
@@ -4451,30 +4451,30 @@
       <c r="C38" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="101" t="s">
+      <c r="D38" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="101"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E38" s="123"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
         <f>SUM(exp_rxns*D30)*0.4</f>
         <v>0</v>
       </c>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
-      <c r="D39" s="112">
+      <c r="D39" s="124">
         <f>SUM(B39*C39)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="112"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E39" s="124"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>338</v>
       </c>
@@ -4490,132 +4490,132 @@
         <v>µl (recommend 1500 ng of product in 30 µl max)</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="99" t="s">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="99"/>
-      <c r="C43" s="99"/>
-      <c r="D43" s="100" t="s">
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="100"/>
-      <c r="I43" s="99" t="s">
+      <c r="E43" s="125"/>
+      <c r="I43" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="99"/>
+      <c r="J43" s="115"/>
       <c r="K43" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="103" t="s">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="103"/>
-      <c r="C44" s="103"/>
-      <c r="D44" s="102">
+      <c r="B44" s="116"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="126">
         <f>IF(B39="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D39)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D39)))</f>
         <v>30</v>
       </c>
-      <c r="E44" s="102"/>
+      <c r="E44" s="126"/>
       <c r="F44" s="5"/>
-      <c r="I44" s="108" t="s">
+      <c r="I44" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="108"/>
+      <c r="J44" s="119"/>
       <c r="K44" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="103" t="s">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="103"/>
-      <c r="C45" s="103"/>
-      <c r="D45" s="102">
+      <c r="B45" s="116"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="126">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D44),"")</f>
         <v>0</v>
       </c>
-      <c r="E45" s="102"/>
+      <c r="E45" s="126"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="103" t="s">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="103"/>
-      <c r="C46" s="103"/>
-      <c r="D46" s="110">
+      <c r="B46" s="116"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="104">
         <v>5</v>
       </c>
-      <c r="E46" s="110"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="103" t="s">
-        <v>388</v>
-      </c>
-      <c r="B47" s="103"/>
-      <c r="C47" s="103"/>
-      <c r="D47" s="110">
+      <c r="E46" s="104"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="116" t="s">
+        <v>385</v>
+      </c>
+      <c r="B47" s="116"/>
+      <c r="C47" s="116"/>
+      <c r="D47" s="104">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E47" s="110"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="103" t="s">
+      <c r="E47" s="104"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="103"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="110">
+      <c r="B48" s="116"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="104">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E48" s="110"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="111">
+      <c r="E48" s="104"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D49" s="128">
         <f>SUM(D44:D48)</f>
         <v>50</v>
       </c>
-      <c r="E49" s="111"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E49" s="128"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C52" s="47"/>
       <c r="D52" s="71" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="109" t="s">
-        <v>391</v>
-      </c>
-      <c r="B53" s="109"/>
-      <c r="C53" s="109"/>
-      <c r="D53" s="109"/>
-      <c r="E53" s="109"/>
-      <c r="F53" s="109"/>
-      <c r="G53" s="109"/>
-      <c r="H53" s="109"/>
-      <c r="I53" s="109"/>
-      <c r="J53" s="109"/>
-      <c r="K53" s="109"/>
-      <c r="L53" s="109"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="131" t="s">
+        <v>388</v>
+      </c>
+      <c r="B53" s="131"/>
+      <c r="C53" s="131"/>
+      <c r="D53" s="131"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="131"/>
+      <c r="H53" s="131"/>
+      <c r="I53" s="131"/>
+      <c r="J53" s="131"/>
+      <c r="K53" s="131"/>
+      <c r="L53" s="131"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="71" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -4628,46 +4628,46 @@
       <c r="K54" s="71"/>
       <c r="L54" s="88"/>
     </row>
-    <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="105" t="s">
+    <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="105"/>
-      <c r="C55" s="105" t="s">
+      <c r="B55" s="113"/>
+      <c r="C55" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="105"/>
-      <c r="E55" s="105" t="s">
+      <c r="D55" s="113"/>
+      <c r="E55" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="F55" s="105"/>
-      <c r="G55" s="105" t="s">
+      <c r="F55" s="113"/>
+      <c r="G55" s="113" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="105"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="106">
+      <c r="H55" s="113"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="129">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B56" s="106"/>
-      <c r="C56" s="107"/>
-      <c r="D56" s="107"/>
-      <c r="E56" s="107"/>
-      <c r="F56" s="107"/>
-      <c r="G56" s="108">
+      <c r="B56" s="129"/>
+      <c r="C56" s="130"/>
+      <c r="D56" s="130"/>
+      <c r="E56" s="130"/>
+      <c r="F56" s="130"/>
+      <c r="G56" s="119">
         <f>SUM(C56*E56)</f>
         <v>0</v>
       </c>
-      <c r="H56" s="108"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H56" s="119"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>338</v>
       </c>
@@ -4678,142 +4678,142 @@
       </c>
       <c r="H59" s="18"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="99" t="s">
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="99"/>
-      <c r="C60" s="99"/>
-      <c r="D60" s="100" t="s">
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="100"/>
-    </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="101" t="s">
+      <c r="E60" s="125"/>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="123" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="101"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="102">
+      <c r="B61" s="123"/>
+      <c r="C61" s="123"/>
+      <c r="D61" s="126">
         <f>IF(C56="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G56)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G56)))</f>
         <v>12</v>
       </c>
-      <c r="E61" s="102"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="101" t="s">
+      <c r="E61" s="126"/>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="101"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="102" t="str">
+      <c r="B62" s="123"/>
+      <c r="C62" s="123"/>
+      <c r="D62" s="126" t="str">
         <f>IFERROR((IF(SUM(12-D61)=0,"-",SUM(12-D61))),"")</f>
         <v>-</v>
       </c>
-      <c r="E62" s="102"/>
-    </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="103" t="s">
-        <v>396</v>
-      </c>
-      <c r="B63" s="103"/>
-      <c r="C63" s="103"/>
-      <c r="D63" s="104">
+      <c r="E62" s="126"/>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="116" t="s">
+        <v>393</v>
+      </c>
+      <c r="B63" s="116"/>
+      <c r="C63" s="116"/>
+      <c r="D63" s="132">
         <v>37.5</v>
       </c>
-      <c r="E63" s="104"/>
-    </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="103" t="s">
-        <v>397</v>
-      </c>
-      <c r="B64" s="103"/>
-      <c r="C64" s="103"/>
-      <c r="D64" s="104">
+      <c r="E63" s="132"/>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="116" t="s">
+        <v>394</v>
+      </c>
+      <c r="B64" s="116"/>
+      <c r="C64" s="116"/>
+      <c r="D64" s="132">
         <v>25.5</v>
       </c>
-      <c r="E64" s="104"/>
+      <c r="E64" s="132"/>
       <c r="F64" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C66" s="5"/>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="95" t="s">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="95"/>
-      <c r="C67" s="97"/>
-      <c r="D67" s="97"/>
+      <c r="B67" s="96"/>
+      <c r="C67" s="134"/>
+      <c r="D67" s="134"/>
       <c r="E67" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="95" t="s">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="95"/>
-      <c r="C68" s="96"/>
-      <c r="D68" s="96"/>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="95" t="s">
+      <c r="B68" s="96"/>
+      <c r="C68" s="133"/>
+      <c r="D68" s="133"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="95"/>
-      <c r="C69" s="96"/>
-      <c r="D69" s="96"/>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="95" t="s">
+      <c r="B69" s="96"/>
+      <c r="C69" s="133"/>
+      <c r="D69" s="133"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="95"/>
-      <c r="C70" s="98" t="str">
+      <c r="B70" s="96"/>
+      <c r="C70" s="135" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D70" s="98"/>
+      <c r="D70" s="135"/>
       <c r="E70" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="95" t="s">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="95"/>
-      <c r="C71" s="97"/>
-      <c r="D71" s="97"/>
+      <c r="B71" s="96"/>
+      <c r="C71" s="134"/>
+      <c r="D71" s="134"/>
       <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="95" t="s">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="95"/>
-      <c r="C72" s="96"/>
-      <c r="D72" s="96"/>
+      <c r="B72" s="96"/>
+      <c r="C72" s="133"/>
+      <c r="D72" s="133"/>
       <c r="E72" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="95" t="s">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="95"/>
-      <c r="C73" s="96"/>
-      <c r="D73" s="96"/>
+      <c r="B73" s="96"/>
+      <c r="C73" s="133"/>
+      <c r="D73" s="133"/>
       <c r="E73" s="9" t="s">
         <v>68</v>
       </c>
@@ -4821,108 +4821,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="116">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="A73:B73"/>
@@ -4937,6 +4835,108 @@
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B59">
     <cfRule type="expression" dxfId="14" priority="7">
@@ -5068,7 +5068,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>reference!$K$3:$K$9</xm:f>
+            <xm:f>reference!$L$3:$L$9</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -5077,7 +5077,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
-            <xm:f>reference!$H$3:$H$9</xm:f>
+            <xm:f>reference!$I$3:$I$9</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>0</xm:f>
@@ -5114,18 +5114,18 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="6.625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="4" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="1" max="2" width="6.59765625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="6.59765625" customWidth="1"/>
+    <col min="4" max="5" width="11.8984375" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.09765625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="13" max="28" width="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C1" s="47"/>
       <c r="D1" s="136" t="s">
         <v>69</v>
@@ -5165,7 +5165,7 @@
       <c r="AE1" s="138"/>
       <c r="AF1" s="138"/>
     </row>
-    <row r="2" spans="1:32" s="15" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:32" s="15" customFormat="1" ht="79.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="49" t="s">
         <v>73</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>76</v>
       </c>
       <c r="F2" s="73" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G2" s="74" t="s">
         <v>77</v>
@@ -5203,34 +5203,34 @@
         <v>82</v>
       </c>
       <c r="M2" s="76" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="N2" s="76" t="s">
         <v>365</v>
       </c>
       <c r="O2" s="76" t="s">
+        <v>407</v>
+      </c>
+      <c r="P2" s="76" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q2" s="76" t="s">
+        <v>416</v>
+      </c>
+      <c r="R2" s="76" t="s">
         <v>410</v>
       </c>
-      <c r="P2" s="76" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q2" s="76" t="s">
-        <v>419</v>
-      </c>
-      <c r="R2" s="76" t="s">
-        <v>413</v>
-      </c>
       <c r="S2" s="76" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="T2" s="76" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="U2" s="76" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="V2" s="76" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="W2" s="76" t="s">
         <v>371</v>
@@ -5239,16 +5239,16 @@
         <v>372</v>
       </c>
       <c r="Y2" s="76" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="Z2" s="76" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="AA2" s="76" t="s">
+        <v>403</v>
+      </c>
+      <c r="AB2" s="76" t="s">
         <v>406</v>
-      </c>
-      <c r="AB2" s="76" t="s">
-        <v>409</v>
       </c>
       <c r="AC2" s="76" t="s">
         <v>368</v>
@@ -5263,7 +5263,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="50">
         <v>1</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59">
         <v>2</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59">
         <v>3</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="59">
         <v>4</v>
       </c>
@@ -5675,7 +5675,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="59">
         <v>5</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="59">
         <v>6</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59">
         <v>7</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="61">
         <v>8</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="50">
         <v>9</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="59">
         <v>10</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59">
         <v>11</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59">
         <v>12</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="59">
         <v>13</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="61">
         <v>16</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
         <v>17</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="59">
         <v>18</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="59">
         <v>19</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="59">
         <v>20</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="59">
         <v>21</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="59">
         <v>22</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="59">
         <v>23</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="61">
         <v>24</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="50">
         <v>25</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="59">
         <v>26</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="59">
         <v>27</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="59">
         <v>28</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="59">
         <v>29</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="59">
         <v>30</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="59">
         <v>31</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="61">
         <v>32</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="50">
         <v>33</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="59">
         <v>34</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="59">
         <v>35</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="59">
         <v>36</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="59">
         <v>37</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="59">
         <v>38</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="59">
         <v>39</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="61">
         <v>40</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
         <v>41</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="59">
         <v>42</v>
       </c>
@@ -9589,7 +9589,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="59">
         <v>43</v>
       </c>
@@ -9692,7 +9692,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="59">
         <v>44</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="59">
         <v>45</v>
       </c>
@@ -9898,7 +9898,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="59">
         <v>46</v>
       </c>
@@ -10001,7 +10001,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="59">
         <v>47</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="61">
         <v>48</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50">
         <v>49</v>
       </c>
@@ -10310,7 +10310,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="59">
         <v>50</v>
       </c>
@@ -10413,7 +10413,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="59">
         <v>51</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="59">
         <v>52</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="59">
         <v>53</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="59">
         <v>54</v>
       </c>
@@ -10825,7 +10825,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="59">
         <v>55</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="61">
         <v>56</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="50">
         <v>57</v>
       </c>
@@ -11134,7 +11134,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="59">
         <v>58</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="59">
         <v>59</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="59">
         <v>60</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="59">
         <v>61</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="59">
         <v>62</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="59">
         <v>63</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="61">
         <v>64</v>
       </c>
@@ -11855,7 +11855,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="50">
         <v>65</v>
       </c>
@@ -11958,7 +11958,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="59">
         <v>66</v>
       </c>
@@ -12061,7 +12061,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="59">
         <v>67</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="59">
         <v>68</v>
       </c>
@@ -12267,7 +12267,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="59">
         <v>69</v>
       </c>
@@ -12370,7 +12370,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="59">
         <v>70</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="59">
         <v>71</v>
       </c>
@@ -12576,7 +12576,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="61">
         <v>72</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="50">
         <v>73</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="59">
         <v>74</v>
       </c>
@@ -12885,7 +12885,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="59">
         <v>75</v>
       </c>
@@ -12988,7 +12988,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="59">
         <v>76</v>
       </c>
@@ -13091,7 +13091,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="59">
         <v>77</v>
       </c>
@@ -13194,7 +13194,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="59">
         <v>78</v>
       </c>
@@ -13297,7 +13297,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="59">
         <v>79</v>
       </c>
@@ -13400,7 +13400,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="61">
         <v>80</v>
       </c>
@@ -13503,7 +13503,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="50">
         <v>81</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="59">
         <v>82</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="59">
         <v>83</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="59">
         <v>84</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="59">
         <v>85</v>
       </c>
@@ -14018,7 +14018,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="59">
         <v>86</v>
       </c>
@@ -14121,7 +14121,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="59">
         <v>87</v>
       </c>
@@ -14224,7 +14224,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="61">
         <v>88</v>
       </c>
@@ -14327,7 +14327,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="50">
         <v>89</v>
       </c>
@@ -14430,7 +14430,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="59">
         <v>90</v>
       </c>
@@ -14533,7 +14533,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="59">
         <v>91</v>
       </c>
@@ -14636,7 +14636,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="59">
         <v>92</v>
       </c>
@@ -14739,7 +14739,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="59">
         <v>93</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="59">
         <v>94</v>
       </c>
@@ -14945,7 +14945,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="59">
         <v>95</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="61">
         <v>96</v>
       </c>
@@ -15151,7 +15151,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:32" s="23" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:32" s="23" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="22"/>
       <c r="B99" s="22"/>
       <c r="C99" s="22"/>
@@ -15161,7 +15161,7 @@
       <c r="G99" s="22"/>
       <c r="H99" s="22"/>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -15170,7 +15170,7 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -15179,7 +15179,7 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -15188,7 +15188,7 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -15197,7 +15197,7 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
     </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -15206,7 +15206,7 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
     </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -15215,7 +15215,7 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -15224,7 +15224,7 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -15233,7 +15233,7 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -15242,7 +15242,7 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -15251,7 +15251,7 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -15260,7 +15260,7 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -15317,28 +15317,28 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.25" customWidth="1"/>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="1" max="1" width="34.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.09765625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="5.125" customWidth="1"/>
-    <col min="8" max="8" width="19.75" customWidth="1"/>
-    <col min="9" max="9" width="8.75" customWidth="1"/>
-    <col min="10" max="10" width="5.5" customWidth="1"/>
-    <col min="11" max="11" width="22.625" customWidth="1"/>
-    <col min="13" max="13" width="17.75" customWidth="1"/>
-    <col min="14" max="14" width="28.875" customWidth="1"/>
+    <col min="7" max="8" width="5.09765625" customWidth="1"/>
+    <col min="9" max="9" width="19.69921875" customWidth="1"/>
+    <col min="10" max="10" width="8.69921875" customWidth="1"/>
+    <col min="11" max="11" width="5.5" customWidth="1"/>
+    <col min="12" max="12" width="22.59765625" customWidth="1"/>
+    <col min="14" max="14" width="17.69921875" customWidth="1"/>
+    <col min="15" max="15" width="28.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="77" t="s">
         <v>283</v>
       </c>
@@ -15348,11 +15348,11 @@
         <v>284</v>
       </c>
       <c r="F1" s="77"/>
-      <c r="H1" s="77" t="s">
+      <c r="I1" s="77" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="78" t="s">
         <v>286</v>
       </c>
@@ -15362,17 +15362,17 @@
         <v>287</v>
       </c>
       <c r="F2" s="80"/>
-      <c r="H2" s="81" t="s">
+      <c r="I2" s="81" t="s">
         <v>288</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="J2" s="81" t="s">
         <v>289</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="L2" s="81" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>292</v>
       </c>
@@ -15386,17 +15386,17 @@
       <c r="E3" t="s">
         <v>291</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="I3" s="35" t="s">
         <v>381</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="J3" s="35" t="s">
         <v>382</v>
       </c>
-      <c r="K3" s="35" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>295</v>
       </c>
@@ -15411,17 +15411,17 @@
       <c r="E4" t="s">
         <v>294</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>393</v>
-      </c>
       <c r="I4" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="J4" s="35" t="s">
         <v>383</v>
       </c>
-      <c r="K4" s="35" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="35" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>298</v>
       </c>
@@ -15431,22 +15431,22 @@
       <c r="C5" t="s">
         <v>293</v>
       </c>
-      <c r="H5" s="35" t="s">
-        <v>394</v>
-      </c>
       <c r="I5" s="35" t="s">
+        <v>391</v>
+      </c>
+      <c r="J5" s="35" t="s">
         <v>384</v>
       </c>
-      <c r="K5" s="35" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="35" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>364</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C6" t="s">
         <v>380</v>
@@ -15455,46 +15455,46 @@
         <v>340</v>
       </c>
       <c r="F6" s="80"/>
-      <c r="H6" s="35"/>
       <c r="I6" s="35"/>
-      <c r="K6" s="35"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J6" s="35"/>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="E7">
         <v>100</v>
       </c>
-      <c r="H7" s="35"/>
       <c r="I7" s="35"/>
-      <c r="K7" s="35"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J7" s="35"/>
+      <c r="L7" s="35"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E8">
         <v>50</v>
       </c>
-      <c r="H8" s="35"/>
       <c r="I8" s="35"/>
-      <c r="K8" s="35"/>
-    </row>
-    <row r="9" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="35"/>
+      <c r="L8" s="35"/>
+    </row>
+    <row r="9" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="78" t="s">
         <v>301</v>
       </c>
       <c r="B9" s="79"/>
       <c r="C9" s="79"/>
-      <c r="H9" s="35"/>
       <c r="I9" s="35"/>
-      <c r="K9" s="35"/>
-    </row>
-    <row r="10" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="35"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>303</v>
       </c>
@@ -15505,11 +15505,11 @@
         <v>356</v>
       </c>
       <c r="F10" s="80"/>
-      <c r="H10" s="82" t="s">
+      <c r="I10" s="82" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>305</v>
       </c>
@@ -15519,74 +15519,75 @@
       <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="82" t="s">
+      <c r="I11" s="82" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>357</v>
       </c>
-      <c r="H12" s="82" t="s">
+      <c r="I12" s="82" t="s">
         <v>299</v>
       </c>
-      <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
-    </row>
-    <row r="13" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="78" t="s">
         <v>336</v>
       </c>
       <c r="E13" t="s">
         <v>358</v>
       </c>
-      <c r="H13" s="82" t="s">
+      <c r="I13" s="82" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E14" t="s">
         <v>359</v>
       </c>
-      <c r="H14" s="82" t="s">
+      <c r="I14" s="82" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E15" s="15" t="s">
         <v>360</v>
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="17" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="79" t="s">
         <v>361</v>
       </c>
       <c r="F17" s="80"/>
     </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>64</v>
       </c>
       <c r="G19" s="15"/>
-    </row>
-    <row r="21" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="15"/>
+    </row>
+    <row r="21" spans="5:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E21" s="83" t="s">
         <v>373</v>
       </c>
       <c r="F21" s="80"/>
     </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E22" s="80" t="s">
         <v>374</v>
       </c>
@@ -15594,7 +15595,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>365</v>
       </c>
@@ -15602,42 +15603,42 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F24" t="s">
         <v>376</v>
       </c>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F25" t="s">
-        <v>416</v>
-      </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>366</v>
       </c>
       <c r="F26" t="s">
-        <v>414</v>
-      </c>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>367</v>
       </c>
       <c r="F27" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>371</v>
       </c>
@@ -15645,7 +15646,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>370</v>
       </c>
@@ -15653,7 +15654,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="30" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>372</v>
       </c>
@@ -15661,13 +15662,13 @@
         <v>379</v>
       </c>
     </row>
-    <row r="32" spans="5:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E32" s="83" t="s">
         <v>373</v>
       </c>
       <c r="F32" s="80"/>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E33" s="80" t="s">
         <v>374</v>
       </c>
@@ -15675,92 +15676,92 @@
         <v>286</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
+        <v>396</v>
+      </c>
+      <c r="F34" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>397</v>
+      </c>
+      <c r="F35" t="s">
         <v>399</v>
       </c>
-      <c r="F34" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>400</v>
-      </c>
-      <c r="F35" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="5:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E37" s="83" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F37" s="80" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E38" s="47">
         <v>700</v>
       </c>
       <c r="F38" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E39" s="47">
         <v>200</v>
       </c>
       <c r="F39" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E41" s="83" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E42" s="47">
         <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E43" s="47">
         <v>70</v>
       </c>
       <c r="F43" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="45" spans="5:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E45" s="94" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
       <formula1>$E$23:$E$30</formula1>
@@ -15782,21 +15783,21 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.875" customWidth="1"/>
+    <col min="1" max="1" width="28.8984375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
-    <col min="4" max="13" width="16.125" customWidth="1"/>
+    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="4" max="13" width="16.09765625" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
-    <col min="15" max="20" width="16.125" customWidth="1"/>
+    <col min="15" max="20" width="16.09765625" customWidth="1"/>
     <col min="21" max="21" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:9" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A1" s="36" t="s">
         <v>341</v>
       </c>
@@ -15809,7 +15810,7 @@
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
     </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A2" s="38" t="s">
         <v>348</v>
       </c>
@@ -15822,7 +15823,7 @@
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A3" s="38"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -15833,7 +15834,7 @@
       <c r="H3" s="37"/>
       <c r="I3" s="37"/>
     </row>
-    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A4" s="39" t="s">
         <v>342</v>
       </c>
@@ -15846,7 +15847,7 @@
       <c r="H4" s="37"/>
       <c r="I4" s="37"/>
     </row>
-    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A5" s="37" t="s">
         <v>343</v>
       </c>
@@ -15859,7 +15860,7 @@
       <c r="H5" s="37"/>
       <c r="I5" s="37"/>
     </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="40" t="s">
         <v>277</v>
       </c>
@@ -15874,7 +15875,7 @@
       <c r="H6" s="37"/>
       <c r="I6" s="37"/>
     </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A7" s="40" t="s">
         <v>278</v>
       </c>
@@ -15889,7 +15890,7 @@
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
     </row>
-    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A8" s="41" t="s">
         <v>280</v>
       </c>
@@ -15904,7 +15905,7 @@
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
     </row>
-    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A9" s="42" t="s">
         <v>281</v>
       </c>
@@ -15919,7 +15920,7 @@
       <c r="H9" s="37"/>
       <c r="I9" s="37"/>
     </row>
-    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A10" s="42" t="s">
         <v>282</v>
       </c>
@@ -15934,7 +15935,7 @@
       <c r="H10" s="37"/>
       <c r="I10" s="37"/>
     </row>
-    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B11" s="38"/>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -15944,7 +15945,7 @@
       <c r="H11" s="37"/>
       <c r="I11" s="37"/>
     </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -15954,7 +15955,7 @@
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
     </row>
-    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A13" s="43" t="s">
         <v>347</v>
       </c>
@@ -15967,7 +15968,7 @@
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
     </row>
-    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A14" s="37" t="s">
         <v>349</v>
       </c>
@@ -15980,7 +15981,7 @@
       <c r="H14" s="37"/>
       <c r="I14" s="37"/>
     </row>
-    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A15" s="38" t="s">
         <v>355</v>
       </c>
@@ -15993,7 +15994,7 @@
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
     </row>
-    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A16" s="38" t="s">
         <v>354</v>
       </c>
@@ -16006,7 +16007,7 @@
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
     </row>
-    <row r="17" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A17" s="38"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -16017,7 +16018,7 @@
       <c r="H17" s="37"/>
       <c r="I17" s="37"/>
     </row>
-    <row r="18" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A18" s="39" t="s">
         <v>353</v>
       </c>
@@ -16030,12 +16031,12 @@
       <c r="H18" s="37"/>
       <c r="I18" s="37"/>
     </row>
-    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A19" s="38" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A20" s="37" t="s">
         <v>350</v>
       </c>
@@ -16057,17 +16058,17 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
-    <col min="3" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="11.75" customWidth="1"/>
-    <col min="10" max="10" width="12.625" customWidth="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" customWidth="1"/>
+    <col min="3" max="7" width="12.09765625" customWidth="1"/>
+    <col min="9" max="9" width="11.69921875" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" customWidth="1"/>
+    <col min="11" max="11" width="16.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="15" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="15" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>306</v>
       </c>
@@ -16108,7 +16109,7 @@
         <v>318</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="O1" s="15" t="s">
         <v>319</v>
@@ -16141,7 +16142,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(LEN(exp_id)=0,"",exp_id)</f>
         <v/>
@@ -16260,17 +16261,17 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.25" customWidth="1"/>
-    <col min="2" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="7" width="11.25" customWidth="1"/>
-    <col min="8" max="8" width="10.75" customWidth="1"/>
-    <col min="9" max="9" width="28.125" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="4" width="13.69921875" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" customWidth="1"/>
+    <col min="6" max="7" width="11.19921875" customWidth="1"/>
+    <col min="8" max="8" width="10.69921875" customWidth="1"/>
+    <col min="9" max="9" width="28.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>329</v>
       </c>
@@ -16278,7 +16279,7 @@
         <v>330</v>
       </c>
       <c r="C1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D1" t="s">
         <v>306</v>
@@ -16299,7 +16300,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(LEN(Library!D3)=0,"",Library!D3)</f>
         <v/>
@@ -16337,7 +16338,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF(LEN(Library!D4)=0,"",Library!D4)</f>
         <v/>
@@ -16375,7 +16376,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF(LEN(Library!D5)=0,"",Library!D5)</f>
         <v/>
@@ -16413,7 +16414,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF(LEN(Library!D6)=0,"",Library!D6)</f>
         <v/>
@@ -16451,7 +16452,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF(LEN(Library!D7)=0,"",Library!D7)</f>
         <v/>
@@ -16489,7 +16490,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF(LEN(Library!D8)=0,"",Library!D8)</f>
         <v/>
@@ -16527,7 +16528,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF(LEN(Library!D9)=0,"",Library!D9)</f>
         <v/>
@@ -16565,7 +16566,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF(LEN(Library!D10)=0,"",Library!D10)</f>
         <v/>
@@ -16603,7 +16604,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF(LEN(Library!D11)=0,"",Library!D11)</f>
         <v/>
@@ -16641,7 +16642,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF(LEN(Library!D12)=0,"",Library!D12)</f>
         <v/>
@@ -16679,7 +16680,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF(LEN(Library!D13)=0,"",Library!D13)</f>
         <v/>
@@ -16717,7 +16718,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(LEN(Library!D14)=0,"",Library!D14)</f>
         <v/>
@@ -16755,7 +16756,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF(LEN(Library!D15)=0,"",Library!D15)</f>
         <v/>
@@ -16793,7 +16794,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF(LEN(Library!D16)=0,"",Library!D16)</f>
         <v/>
@@ -16831,7 +16832,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF(LEN(Library!D17)=0,"",Library!D17)</f>
         <v/>
@@ -16869,7 +16870,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF(LEN(Library!D18)=0,"",Library!D18)</f>
         <v/>
@@ -16907,7 +16908,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF(LEN(Library!D19)=0,"",Library!D19)</f>
         <v/>
@@ -16945,7 +16946,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF(LEN(Library!D20)=0,"",Library!D20)</f>
         <v/>
@@ -16983,7 +16984,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF(LEN(Library!D21)=0,"",Library!D21)</f>
         <v/>
@@ -17021,7 +17022,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF(LEN(Library!D22)=0,"",Library!D22)</f>
         <v/>
@@ -17059,7 +17060,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF(LEN(Library!D23)=0,"",Library!D23)</f>
         <v/>
@@ -17097,7 +17098,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF(LEN(Library!D24)=0,"",Library!D24)</f>
         <v/>
@@ -17135,7 +17136,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF(LEN(Library!D25)=0,"",Library!D25)</f>
         <v/>
@@ -17173,7 +17174,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF(LEN(Library!D26)=0,"",Library!D26)</f>
         <v/>
@@ -17211,7 +17212,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF(LEN(Library!D27)=0,"",Library!D27)</f>
         <v/>
@@ -17249,7 +17250,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF(LEN(Library!D28)=0,"",Library!D28)</f>
         <v/>
@@ -17287,7 +17288,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF(LEN(Library!D29)=0,"",Library!D29)</f>
         <v/>
@@ -17325,7 +17326,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF(LEN(Library!D30)=0,"",Library!D30)</f>
         <v/>
@@ -17363,7 +17364,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF(LEN(Library!D31)=0,"",Library!D31)</f>
         <v/>
@@ -17401,7 +17402,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF(LEN(Library!D32)=0,"",Library!D32)</f>
         <v/>
@@ -17439,7 +17440,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF(LEN(Library!D33)=0,"",Library!D33)</f>
         <v/>
@@ -17477,7 +17478,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF(LEN(Library!D34)=0,"",Library!D34)</f>
         <v/>
@@ -17515,7 +17516,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF(LEN(Library!D35)=0,"",Library!D35)</f>
         <v/>
@@ -17553,7 +17554,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF(LEN(Library!D36)=0,"",Library!D36)</f>
         <v/>
@@ -17591,7 +17592,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF(LEN(Library!D37)=0,"",Library!D37)</f>
         <v/>
@@ -17629,7 +17630,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF(LEN(Library!D38)=0,"",Library!D38)</f>
         <v/>
@@ -17667,7 +17668,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF(LEN(Library!D39)=0,"",Library!D39)</f>
         <v/>
@@ -17705,7 +17706,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF(LEN(Library!D40)=0,"",Library!D40)</f>
         <v/>
@@ -17743,7 +17744,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF(LEN(Library!D41)=0,"",Library!D41)</f>
         <v/>
@@ -17781,7 +17782,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF(LEN(Library!D42)=0,"",Library!D42)</f>
         <v/>
@@ -17819,7 +17820,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF(LEN(Library!D43)=0,"",Library!D43)</f>
         <v/>
@@ -17857,7 +17858,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF(LEN(Library!D44)=0,"",Library!D44)</f>
         <v/>
@@ -17895,7 +17896,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF(LEN(Library!D45)=0,"",Library!D45)</f>
         <v/>
@@ -17933,7 +17934,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF(LEN(Library!D46)=0,"",Library!D46)</f>
         <v/>
@@ -17971,7 +17972,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF(LEN(Library!D47)=0,"",Library!D47)</f>
         <v/>
@@ -18009,7 +18010,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF(LEN(Library!D48)=0,"",Library!D48)</f>
         <v/>
@@ -18047,7 +18048,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF(LEN(Library!D49)=0,"",Library!D49)</f>
         <v/>
@@ -18085,7 +18086,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF(LEN(Library!D50)=0,"",Library!D50)</f>
         <v/>
@@ -18123,7 +18124,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF(LEN(Library!D51)=0,"",Library!D51)</f>
         <v/>
@@ -18161,7 +18162,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF(LEN(Library!D52)=0,"",Library!D52)</f>
         <v/>
@@ -18199,7 +18200,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF(LEN(Library!D53)=0,"",Library!D53)</f>
         <v/>
@@ -18237,7 +18238,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF(LEN(Library!D54)=0,"",Library!D54)</f>
         <v/>
@@ -18275,7 +18276,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF(LEN(Library!D55)=0,"",Library!D55)</f>
         <v/>
@@ -18313,7 +18314,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF(LEN(Library!D56)=0,"",Library!D56)</f>
         <v/>
@@ -18351,7 +18352,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>IF(LEN(Library!D57)=0,"",Library!D57)</f>
         <v/>
@@ -18389,7 +18390,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="str">
         <f>IF(LEN(Library!D58)=0,"",Library!D58)</f>
         <v/>
@@ -18427,7 +18428,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f>IF(LEN(Library!D59)=0,"",Library!D59)</f>
         <v/>
@@ -18465,7 +18466,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f>IF(LEN(Library!D60)=0,"",Library!D60)</f>
         <v/>
@@ -18503,7 +18504,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f>IF(LEN(Library!D61)=0,"",Library!D61)</f>
         <v/>
@@ -18541,7 +18542,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f>IF(LEN(Library!D62)=0,"",Library!D62)</f>
         <v/>
@@ -18579,7 +18580,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="str">
         <f>IF(LEN(Library!D63)=0,"",Library!D63)</f>
         <v/>
@@ -18617,7 +18618,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="str">
         <f>IF(LEN(Library!D64)=0,"",Library!D64)</f>
         <v/>
@@ -18655,7 +18656,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="str">
         <f>IF(LEN(Library!D65)=0,"",Library!D65)</f>
         <v/>
@@ -18693,7 +18694,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="str">
         <f>IF(LEN(Library!D66)=0,"",Library!D66)</f>
         <v/>
@@ -18731,7 +18732,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="str">
         <f>IF(LEN(Library!D67)=0,"",Library!D67)</f>
         <v/>
@@ -18769,7 +18770,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="str">
         <f>IF(LEN(Library!D68)=0,"",Library!D68)</f>
         <v/>
@@ -18807,7 +18808,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
         <f>IF(LEN(Library!D69)=0,"",Library!D69)</f>
         <v/>
@@ -18845,7 +18846,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="str">
         <f>IF(LEN(Library!D70)=0,"",Library!D70)</f>
         <v/>
@@ -18883,7 +18884,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f>IF(LEN(Library!D71)=0,"",Library!D71)</f>
         <v/>
@@ -18921,7 +18922,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="str">
         <f>IF(LEN(Library!D72)=0,"",Library!D72)</f>
         <v/>
@@ -18959,7 +18960,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="str">
         <f>IF(LEN(Library!D73)=0,"",Library!D73)</f>
         <v/>
@@ -18997,7 +18998,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="str">
         <f>IF(LEN(Library!D74)=0,"",Library!D74)</f>
         <v/>
@@ -19035,7 +19036,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="str">
         <f>IF(LEN(Library!D75)=0,"",Library!D75)</f>
         <v/>
@@ -19073,7 +19074,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="str">
         <f>IF(LEN(Library!D76)=0,"",Library!D76)</f>
         <v/>
@@ -19111,7 +19112,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="str">
         <f>IF(LEN(Library!D77)=0,"",Library!D77)</f>
         <v/>
@@ -19149,7 +19150,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="str">
         <f>IF(LEN(Library!D78)=0,"",Library!D78)</f>
         <v/>
@@ -19187,7 +19188,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="str">
         <f>IF(LEN(Library!D79)=0,"",Library!D79)</f>
         <v/>
@@ -19225,7 +19226,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="str">
         <f>IF(LEN(Library!D80)=0,"",Library!D80)</f>
         <v/>
@@ -19263,7 +19264,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="str">
         <f>IF(LEN(Library!D81)=0,"",Library!D81)</f>
         <v/>
@@ -19301,7 +19302,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="str">
         <f>IF(LEN(Library!D82)=0,"",Library!D82)</f>
         <v/>
@@ -19339,7 +19340,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="str">
         <f>IF(LEN(Library!D83)=0,"",Library!D83)</f>
         <v/>
@@ -19377,7 +19378,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="str">
         <f>IF(LEN(Library!D84)=0,"",Library!D84)</f>
         <v/>
@@ -19415,7 +19416,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="str">
         <f>IF(LEN(Library!D85)=0,"",Library!D85)</f>
         <v/>
@@ -19453,7 +19454,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="str">
         <f>IF(LEN(Library!D86)=0,"",Library!D86)</f>
         <v/>
@@ -19491,7 +19492,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="str">
         <f>IF(LEN(Library!D87)=0,"",Library!D87)</f>
         <v/>
@@ -19529,7 +19530,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="str">
         <f>IF(LEN(Library!D88)=0,"",Library!D88)</f>
         <v/>
@@ -19567,7 +19568,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="str">
         <f>IF(LEN(Library!D89)=0,"",Library!D89)</f>
         <v/>
@@ -19605,7 +19606,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="str">
         <f>IF(LEN(Library!D90)=0,"",Library!D90)</f>
         <v/>
@@ -19643,7 +19644,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="str">
         <f>IF(LEN(Library!D91)=0,"",Library!D91)</f>
         <v/>
@@ -19681,7 +19682,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="str">
         <f>IF(LEN(Library!D92)=0,"",Library!D92)</f>
         <v/>
@@ -19719,7 +19720,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="str">
         <f>IF(LEN(Library!D93)=0,"",Library!D93)</f>
         <v/>
@@ -19757,7 +19758,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="str">
         <f>IF(LEN(Library!D94)=0,"",Library!D94)</f>
         <v/>
@@ -19795,7 +19796,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="str">
         <f>IF(LEN(Library!D95)=0,"",Library!D95)</f>
         <v/>
@@ -19833,7 +19834,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="str">
         <f>IF(LEN(Library!D96)=0,"",Library!D96)</f>
         <v/>
@@ -19871,7 +19872,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="str">
         <f>IF(LEN(Library!D97)=0,"",Library!D97)</f>
         <v/>
@@ -19909,7 +19910,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="str">
         <f>IF(LEN(Library!D98)=0,"",Library!D98)</f>
         <v/>

</xml_diff>

<commit_message>
Minor updates to template conditional formatting
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1D759C-D272-47AA-BDC8-1B72C3D31CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAB3991-519E-464C-95BD-5182E8321551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="23280" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23508" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,9 @@
     <definedName name="exp_notes">Assay!$C$12</definedName>
     <definedName name="exp_rxns">Assay!$C$11</definedName>
     <definedName name="exp_summary">Assay!$C$9</definedName>
-    <definedName name="exp_type">reference!$B$10</definedName>
+    <definedName name="exp_type">reference!$B$11</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
-    <definedName name="exp_version">reference!$B$11</definedName>
+    <definedName name="exp_version">reference!$B$12</definedName>
     <definedName name="flowcell_checkpores">Assay!$C$72</definedName>
     <definedName name="flowcell_chemisty">Assay!$C$71</definedName>
     <definedName name="flowcell_id">Assay!$C$68</definedName>
@@ -45,9 +45,10 @@
     <definedName name="flowcell_targetmass">Assay!$B$59</definedName>
     <definedName name="flowcell_usage_hrs">Assay!$C$70</definedName>
     <definedName name="library_washbuffer">Assay!$C$52</definedName>
-    <definedName name="missing_qc_resolution">reference!$B$7</definedName>
+    <definedName name="Minimum_final_pooled_DNA_conc">reference!$B$6</definedName>
+    <definedName name="missing_qc_resolution">reference!$B$8</definedName>
     <definedName name="seq_platform">Assay!$C$67</definedName>
-    <definedName name="vol_calc">reference!$B$6</definedName>
+    <definedName name="vol_calc">reference!$B$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="447">
   <si>
     <t>Date:</t>
   </si>
@@ -1746,6 +1747,12 @@
   </si>
   <si>
     <t>Project C</t>
+  </si>
+  <si>
+    <t>Minimum final pooled [DNA]</t>
+  </si>
+  <si>
+    <t>ng/ul</t>
   </si>
 </sst>
 </file>
@@ -3868,7 +3875,7 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4002,7 +4009,7 @@
       <c r="D8" s="108"/>
       <c r="E8" s="108"/>
       <c r="F8" s="108"/>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4671,7 +4678,9 @@
       <c r="A59" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B59" s="28"/>
+      <c r="B59" s="28">
+        <v>800</v>
+      </c>
       <c r="C59" s="9" t="str">
         <f>CONCATENATE("ng of library (max volume = ", flowcell_maxvol,"µl), recommend 800 ng")</f>
         <v>ng of library (max volume = 12µl), recommend 800 ng</v>
@@ -4989,14 +4998,6 @@
       <formula>COUNTIF(F42,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="lessThan">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experimental Aim" error="The aim must be 5-20 characters long as it is used to name folders downstream so can not be too verbose." sqref="C9:F9 C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
@@ -5034,6 +5035,35 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>C70</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="13" operator="lessThan" id="{F2961990-09EF-4874-8343-75AA7400F7E9}">
+            <xm:f>reference!$B$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="14" operator="greaterThanOrEqual" id="{D1C1E73E-7899-481F-B6F9-19D5EC385B53}">
+            <xm:f>reference!$B$6</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G56</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15320,7 +15350,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15400,7 +15430,7 @@
       <c r="A4" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4">
         <f>IF(adaptlig_rxn_vol=100,65,30)</f>
         <v>30</v>
       </c>
@@ -15443,13 +15473,14 @@
     </row>
     <row r="6" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>417</v>
+        <v>445</v>
+      </c>
+      <c r="B6">
+        <f>ROUND(SUM(flowcell_targetmass/flowcell_maxvol),0)</f>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>380</v>
+        <v>446</v>
       </c>
       <c r="E6" s="79" t="s">
         <v>340</v>
@@ -15461,13 +15492,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>396</v>
+        <v>417</v>
       </c>
       <c r="C7" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -15477,6 +15508,15 @@
       <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="C8" t="s">
+        <v>401</v>
+      </c>
       <c r="E8">
         <v>50</v>
       </c>
@@ -15484,23 +15524,17 @@
       <c r="J8" s="35"/>
       <c r="L8" s="35"/>
     </row>
-    <row r="9" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="78" t="s">
-        <v>301</v>
-      </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" t="s">
-        <v>304</v>
-      </c>
+      <c r="A10" s="78" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
       <c r="E10" s="79" t="s">
         <v>356</v>
       </c>
@@ -15511,10 +15545,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
+        <v>304</v>
       </c>
       <c r="E11" t="s">
         <v>58</v>
@@ -15524,6 +15558,12 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
       <c r="E12" t="s">
         <v>357</v>
       </c>
@@ -15535,10 +15575,7 @@
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
     </row>
-    <row r="13" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="78" t="s">
-        <v>336</v>
-      </c>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>358</v>
       </c>
@@ -15546,9 +15583,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>438</v>
+    <row r="14" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="78" t="s">
+        <v>336</v>
       </c>
       <c r="E14" t="s">
         <v>359</v>
@@ -15558,6 +15595,9 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>438</v>
+      </c>
       <c r="E15" s="15" t="s">
         <v>360</v>
       </c>
@@ -15761,12 +15801,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
       <formula1>$E$23:$E$30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{BFF87161-9E78-439F-9B63-F620B9F8A837}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{BFF87161-9E78-439F-9B63-F620B9F8A837}">
       <formula1>$E$34:$E$35</formula1>
     </dataValidation>
   </dataValidations>
@@ -15783,7 +15823,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -16207,9 +16247,9 @@
         <f>IF(LEN(seq_platform)=0,"",seq_platform)</f>
         <v/>
       </c>
-      <c r="Q2" t="str">
+      <c r="Q2">
         <f>IF(LEN(flowcell_targetmass)=0,"",flowcell_targetmass)</f>
-        <v/>
+        <v>800</v>
       </c>
       <c r="R2">
         <f>IF(LEN(flowcell_maxvol)=0,"",flowcell_maxvol)</f>

</xml_diff>

<commit_message>
Added post-pcr conditional formatting of DNA conc
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Ligation_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Ligation_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAB3991-519E-464C-95BD-5182E8321551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47788F03-EF17-41F0-B843-C5B0B27AAE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23508" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,9 @@
     <definedName name="exp_notes">Assay!$C$12</definedName>
     <definedName name="exp_rxns">Assay!$C$11</definedName>
     <definedName name="exp_summary">Assay!$C$9</definedName>
-    <definedName name="exp_type">reference!$B$11</definedName>
+    <definedName name="exp_type">reference!$B$12</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
-    <definedName name="exp_version">reference!$B$12</definedName>
+    <definedName name="exp_version">reference!$B$13</definedName>
     <definedName name="flowcell_checkpores">Assay!$C$72</definedName>
     <definedName name="flowcell_chemisty">Assay!$C$71</definedName>
     <definedName name="flowcell_id">Assay!$C$68</definedName>
@@ -46,9 +46,9 @@
     <definedName name="flowcell_usage_hrs">Assay!$C$70</definedName>
     <definedName name="library_washbuffer">Assay!$C$52</definedName>
     <definedName name="Minimum_final_pooled_DNA_conc">reference!$B$6</definedName>
-    <definedName name="missing_qc_resolution">reference!$B$8</definedName>
+    <definedName name="missing_qc_resolution">reference!$B$9</definedName>
     <definedName name="seq_platform">Assay!$C$67</definedName>
-    <definedName name="vol_calc">reference!$B$7</definedName>
+    <definedName name="vol_calc">reference!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="448">
   <si>
     <t>Date:</t>
   </si>
@@ -1754,6 +1754,9 @@
   <si>
     <t>ng/ul</t>
   </si>
+  <si>
+    <t>Post-PCR clean-up target [DNA]</t>
+  </si>
 </sst>
 </file>
 
@@ -1763,13 +1766,20 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2326,14 +2336,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2353,7 +2363,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2362,16 +2372,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2386,7 +2396,7 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2400,18 +2410,18 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2435,7 +2445,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2446,20 +2456,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2478,7 +2488,7 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2559,38 +2569,38 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2603,7 +2613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2625,125 +2635,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2757,18 +2651,135 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2779,7 +2790,14 @@
     <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="47">
+  <dxfs count="48">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3510,76 +3528,76 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_SeqLib" displayName="tbl_SeqLib" ref="A2:AF98" totalsRowShown="0">
   <autoFilter ref="A2:AF98" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="46"/>
-    <tableColumn id="16" xr3:uid="{D11167BC-CEB0-4BCF-918C-7AFD807B17A9}" name="Column" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{D11167BC-CEB0-4BCF-918C-7AFD807B17A9}" name="Column" dataDxfId="46">
       <calculatedColumnFormula>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Extraction ID" dataDxfId="42"/>
-    <tableColumn id="27" xr3:uid="{D655D6C8-1850-4AC0-8484-17625A62737D}" name="Sample Type" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sWGA Identifier" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PCR Identifier" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PCR Dilution Factor" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Well" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sample ID" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Extraction ID" dataDxfId="43"/>
+    <tableColumn id="27" xr3:uid="{D655D6C8-1850-4AC0-8484-17625A62737D}" name="Sample Type" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sWGA Identifier" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PCR Identifier" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Qubit PCR [DNA] (ng/µl)" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PCR Dilution Factor" dataDxfId="38"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PCR [DNA] (ng / µl)"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="36"/>
-    <tableColumn id="26" xr3:uid="{F1EFF32A-7BE1-415D-A6C1-EB6298E86B67}" name="entry" dataDxfId="35">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Barcode#" dataDxfId="37"/>
+    <tableColumn id="26" xr3:uid="{F1EFF32A-7BE1-415D-A6C1-EB6298E86B67}" name="entry" dataDxfId="36">
       <calculatedColumnFormula>IF(OR(ISBLANK(tbl_SeqLib[[#This Row],[Sample ID]]),ISBLANK(endrepair_targetmass)),0,IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,1,2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{001B4B8A-7DCB-4BB4-B720-5DA9C2A7387A}" name="Exact" dataDxfId="34">
+    <tableColumn id="14" xr3:uid="{001B4B8A-7DCB-4BB4-B720-5DA9C2A7387A}" name="Exact" dataDxfId="35">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]&lt;2,"",IF(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(endrepair_targetmass/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{93494231-5E3B-4D67-8106-A21E3E62E444}" name="Min for col" dataDxfId="33">
+    <tableColumn id="19" xr3:uid="{93494231-5E3B-4D67-8106-A21E3E62E444}" name="Min for col" dataDxfId="34">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDUP(_xlfn.MINIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{1FEA1346-E871-470E-AA2A-C8AFB0F9A249}" name="Max for col" dataDxfId="32">
+    <tableColumn id="20" xr3:uid="{1FEA1346-E871-470E-AA2A-C8AFB0F9A249}" name="Max for col" dataDxfId="33">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDDOWN(_xlfn.MAXIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{6A9EBE31-586B-4F64-B082-46847B0D6428}" name="Avg for col" dataDxfId="31">
+    <tableColumn id="21" xr3:uid="{6A9EBE31-586B-4F64-B082-46847B0D6428}" name="Avg for col" dataDxfId="32">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,ROUNDUP(AVERAGEIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{D59FA2D5-564A-45ED-A2E9-851026B8F744}" name="3 per col" dataDxfId="30">
+    <tableColumn id="25" xr3:uid="{D59FA2D5-564A-45ED-A2E9-851026B8F744}" name="3 per col" dataDxfId="31">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Min for col]:[Avg for col]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Min for col]:[Avg for col]],"",1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{BAABBDBE-05B7-486D-848A-EDB46E768A26}" name="2 per col" dataDxfId="29">
+    <tableColumn id="17" xr3:uid="{BAABBDBE-05B7-486D-848A-EDB46E768A26}" name="2 per col" dataDxfId="30">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Max for col]:[Avg for col]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Max for col]:[Avg for col]],"",1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FEDA3D60-A493-4564-992B-620C2DCBD54F}" name="1 per col (max)" dataDxfId="28">
+    <tableColumn id="18" xr3:uid="{FEDA3D60-A493-4564-992B-620C2DCBD54F}" name="1 per col (max)" dataDxfId="29">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Max for col]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{B52F91B1-8FA3-4813-9699-EE87E0A73E1F}" name="1 per col (avg)" dataDxfId="27">
+    <tableColumn id="34" xr3:uid="{B52F91B1-8FA3-4813-9699-EE87E0A73E1F}" name="1 per col (avg)" dataDxfId="28">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Avg for col]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{3DBE046E-BBA1-40FE-9D15-A56B3030C6C7}" name="Avg per plate" dataDxfId="26">
+    <tableColumn id="22" xr3:uid="{3DBE046E-BBA1-40FE-9D15-A56B3030C6C7}" name="Avg per plate" dataDxfId="27">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,AVERAGE(tbl_SeqLib[Exact]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{C00DCD81-1FEF-4ABB-8CC7-499C0C2570E9}" name="Max per plate" dataDxfId="25">
+    <tableColumn id="23" xr3:uid="{C00DCD81-1FEF-4ABB-8CC7-499C0C2570E9}" name="Max per plate" dataDxfId="26">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=2,MAX(tbl_SeqLib[Exact]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{5078A409-FC75-4147-9A85-9D0F799A65C0}" name="2 per plate" dataDxfId="24">
+    <tableColumn id="24" xr3:uid="{5078A409-FC75-4147-9A85-9D0F799A65C0}" name="2 per plate" dataDxfId="25">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(0,ABS(tbl_SeqLib[[#This Row],[Avg per plate]:[Max per plate]]-tbl_SeqLib[[#This Row],[Exact]]),tbl_SeqLib[[#This Row],[Avg per plate]:[Max per plate]],,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{B05461DD-A312-4983-ABE1-1FB7EFDBEC61}" name="Quantified" dataDxfId="23">
+    <tableColumn id="32" xr3:uid="{B05461DD-A312-4983-ABE1-1FB7EFDBEC61}" name="Quantified" dataDxfId="24">
       <calculatedColumnFormula>IF(vol_calc=reference!$E$23,tbl_SeqLib[[#This Row],[Exact]],IF(vol_calc=reference!$E$24,tbl_SeqLib[[#This Row],[1 per col (max)]],IF(vol_calc=reference!$E$25,tbl_SeqLib[[#This Row],[1 per col (avg)]],IF(vol_calc=reference!$E$26,tbl_SeqLib[[#This Row],[2 per col]],IF(vol_calc=reference!$E$27,tbl_SeqLib[[#This Row],[3 per col]],IF(vol_calc=reference!$E$28,tbl_SeqLib[[#This Row],[Max per plate]],IF(vol_calc=reference!$E$29,tbl_SeqLib[[#This Row],[Avg per plate]],IF(vol_calc=reference!$E$30,tbl_SeqLib[[#This Row],[2 per plate]],"ERROR"))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{31A406DE-6554-495B-953B-40F9644FB053}" name="Avg per plate (missing)" dataDxfId="22">
+    <tableColumn id="30" xr3:uid="{31A406DE-6554-495B-953B-40F9644FB053}" name="Avg per plate (missing)" dataDxfId="23">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=1,ROUNDUP(AVERAGE(tbl_SeqLib[Exact]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{C102ACE7-217E-4DB5-BABC-91C1DAD8AB2B}" name="Avg per col (missing)" dataDxfId="21">
+    <tableColumn id="29" xr3:uid="{C102ACE7-217E-4DB5-BABC-91C1DAD8AB2B}" name="Avg per col (missing)" dataDxfId="22">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=1,ROUNDUP(AVERAGEIFS(tbl_SeqLib[Exact],tbl_SeqLib[Column],tbl_SeqLib[[#This Row],[Column]]),1),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{EF7D6D48-AEC3-450E-B0D6-BDE3BF99E719}" name="Not quantified" dataDxfId="20">
+    <tableColumn id="33" xr3:uid="{EF7D6D48-AEC3-450E-B0D6-BDE3BF99E719}" name="Not quantified" dataDxfId="21">
       <calculatedColumnFormula>IF(missing_qc_resolution=reference!$E$34,tbl_SeqLib[[#This Row],[Avg per col (missing)]],tbl_SeqLib[[#This Row],[Avg per plate (missing)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PCR prodct (µl) to add for end-repair (calculated)" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="PCR prodct (µl) to add for end-repair (calculated)" dataDxfId="20">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=0,"",IF(tbl_SeqLib[[#This Row],[entry]]=1,tbl_SeqLib[[#This Row],[Not quantified]],IF(tbl_SeqLib[[#This Row],[entry]]=2,tbl_SeqLib[[#This Row],[Quantified]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{22CC5A4D-2B43-425F-9880-9E27A697A4AC}" name="PCR prodct (µl) added (if different from calculated)" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NF H20 (µl)" dataDxfId="17">
+    <tableColumn id="15" xr3:uid="{22CC5A4D-2B43-425F-9880-9E27A697A4AC}" name="PCR prodct (µl) added (if different from calculated)" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="NF H20 (µl)" dataDxfId="18">
       <calculatedColumnFormula>IF(tbl_SeqLib[[#This Row],[entry]]=0,"",SUM(endrepair_maxvol-IF(tbl_SeqLib[[#This Row],[PCR prodct (µl) added (if different from calculated)]]&gt;0,tbl_SeqLib[[#This Row],[PCR prodct (µl) added (if different from calculated)]],tbl_SeqLib[[#This Row],[PCR prodct (µl) to add for end-repair (calculated)]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SeqLib Identifier" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SeqLib Identifier" dataDxfId="17">
       <calculatedColumnFormula>IF(ISBLANK(tbl_SeqLib[[#This Row],[sWGA Identifier]]),"",CONCATENATE(exp_id,"_",tbl_SeqLib[[#This Row],[Well]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3674,7 +3692,7 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="sample_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="extraction_id"/>
-    <tableColumn id="9" xr3:uid="{C321884E-D42D-45E4-BC5D-30F682C7C762}" name="sample_type" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{C321884E-D42D-45E4-BC5D-30F682C7C762}" name="sample_type" dataDxfId="16">
       <calculatedColumnFormula>IF(LEN(Library!F3)=0,"",Library!F3)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="expt_id"/>
@@ -3884,171 +3902,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="130" t="s">
         <v>392</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="98" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="114" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="J2" s="99" t="s">
+      <c r="H2" s="114"/>
+      <c r="J2" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="99"/>
+      <c r="K2" s="132"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="101"/>
+      <c r="K3" s="134"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="102" t="s">
+      <c r="J4" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="102"/>
+      <c r="K4" s="135"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="125" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="104" t="str">
+      <c r="B5" s="125"/>
+      <c r="C5" s="110" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!I3:J9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="105" t="s">
+      <c r="J5" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="105"/>
+      <c r="K5" s="126"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="103"/>
-      <c r="C6" s="106" t="str">
+      <c r="B6" s="125"/>
+      <c r="C6" s="127" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="106"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="107"/>
-      <c r="C7" s="108"/>
-      <c r="D7" s="108"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
+      <c r="B7" s="128"/>
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="128" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="107"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
       <c r="G8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="109"/>
-      <c r="C9" s="110" t="str">
+      <c r="B9" s="121"/>
+      <c r="C9" s="122" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="109"/>
-      <c r="C10" s="110" t="str">
+      <c r="B10" s="121"/>
+      <c r="C10" s="122" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="96"/>
+      <c r="B11" s="95"/>
       <c r="C11" s="27"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -4056,32 +4074,32 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
@@ -4092,11 +4110,11 @@
       </c>
       <c r="C15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="112" t="s">
+      <c r="I15" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -4126,119 +4144,119 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="113" t="s">
+      <c r="A18" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="113"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="114" t="s">
+      <c r="B18" s="105"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114" t="str">
+      <c r="E18" s="120"/>
+      <c r="F18" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="I18" s="115" t="s">
+      <c r="G18" s="120"/>
+      <c r="I18" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="115"/>
+      <c r="J18" s="99"/>
       <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="117" t="s">
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
+      <c r="D19" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="117"/>
-      <c r="F19" s="118" t="s">
+      <c r="E19" s="115"/>
+      <c r="F19" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="118"/>
-      <c r="I19" s="119">
+      <c r="G19" s="116"/>
+      <c r="I19" s="108">
         <v>20</v>
       </c>
-      <c r="J19" s="119"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="116" t="s">
+      <c r="A20" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="117" t="str">
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="115" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="117"/>
-      <c r="F20" s="118" t="s">
+      <c r="E20" s="115"/>
+      <c r="F20" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="118"/>
-      <c r="I20" s="119">
+      <c r="G20" s="116"/>
+      <c r="I20" s="108">
         <v>65</v>
       </c>
-      <c r="J20" s="119"/>
+      <c r="J20" s="108"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="120">
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="118">
         <v>1.4</v>
       </c>
-      <c r="E21" s="120"/>
-      <c r="F21" s="118">
+      <c r="E21" s="118"/>
+      <c r="F21" s="116">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="118"/>
-      <c r="I21" s="119">
+      <c r="G21" s="116"/>
+      <c r="I21" s="108">
         <v>4</v>
       </c>
-      <c r="J21" s="119"/>
+      <c r="J21" s="108"/>
       <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="120">
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="118">
         <v>0.6</v>
       </c>
-      <c r="E22" s="120"/>
-      <c r="F22" s="118">
+      <c r="E22" s="118"/>
+      <c r="F22" s="116">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>0</v>
       </c>
-      <c r="G22" s="118"/>
+      <c r="G22" s="116"/>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
-      <c r="D23" s="121">
+      <c r="D23" s="119">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="121"/>
+      <c r="E23" s="119"/>
       <c r="F23" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -4263,103 +4281,103 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="113"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="114" t="s">
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114" t="str">
+      <c r="E26" s="120"/>
+      <c r="F26" s="120" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x (µl)</v>
       </c>
-      <c r="G26" s="114"/>
-      <c r="I26" s="115" t="s">
+      <c r="G26" s="120"/>
+      <c r="I26" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="115"/>
+      <c r="J26" s="99"/>
       <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="117">
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="115">
         <v>0.5</v>
       </c>
-      <c r="E27" s="117"/>
-      <c r="F27" s="118" t="s">
+      <c r="E27" s="115"/>
+      <c r="F27" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="118"/>
-      <c r="I27" s="119">
+      <c r="G27" s="116"/>
+      <c r="I27" s="108">
         <v>20</v>
       </c>
-      <c r="J27" s="119"/>
+      <c r="J27" s="108"/>
       <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="117">
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="115">
         <v>6</v>
       </c>
-      <c r="E28" s="117"/>
-      <c r="F28" s="118">
+      <c r="E28" s="115"/>
+      <c r="F28" s="116">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G28" s="118"/>
-      <c r="I28" s="119">
+      <c r="G28" s="116"/>
+      <c r="I28" s="108">
         <v>65</v>
       </c>
-      <c r="J28" s="119"/>
+      <c r="J28" s="108"/>
       <c r="K28" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="117">
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="115">
         <v>0.2</v>
       </c>
-      <c r="E29" s="117"/>
-      <c r="F29" s="118">
+      <c r="E29" s="115"/>
+      <c r="F29" s="116">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>0</v>
       </c>
-      <c r="G29" s="118"/>
-      <c r="I29" s="119">
+      <c r="G29" s="116"/>
+      <c r="I29" s="108">
         <v>8</v>
       </c>
-      <c r="J29" s="119"/>
+      <c r="J29" s="108"/>
       <c r="K29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
-      <c r="D30" s="122">
+      <c r="D30" s="117">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="122"/>
+      <c r="E30" s="117"/>
       <c r="F30" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -4423,19 +4441,19 @@
       <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="127" t="s">
+      <c r="A36" s="113" t="s">
         <v>428</v>
       </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114"/>
+      <c r="F36" s="114"/>
+      <c r="G36" s="114"/>
+      <c r="H36" s="114"/>
+      <c r="I36" s="114"/>
+      <c r="J36" s="114"/>
+      <c r="K36" s="114"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="71" t="s">
@@ -4458,10 +4476,10 @@
       <c r="C38" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="123" t="s">
+      <c r="D38" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="123"/>
+      <c r="E38" s="101"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
@@ -4470,11 +4488,11 @@
       </c>
       <c r="B39" s="34"/>
       <c r="C39" s="34"/>
-      <c r="D39" s="124">
+      <c r="D39" s="112">
         <f>SUM(B39*C39)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="124"/>
+      <c r="E39" s="112"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
@@ -4498,97 +4516,97 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="115" t="s">
+      <c r="A43" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="115"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="125" t="s">
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="125"/>
-      <c r="I43" s="115" t="s">
+      <c r="E43" s="100"/>
+      <c r="I43" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="115"/>
+      <c r="J43" s="99"/>
       <c r="K43" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="116" t="s">
+      <c r="A44" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="116"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="126">
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="102">
         <f>IF(B39="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D39)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D39)))</f>
         <v>30</v>
       </c>
-      <c r="E44" s="126"/>
+      <c r="E44" s="102"/>
       <c r="F44" s="5"/>
-      <c r="I44" s="119" t="s">
+      <c r="I44" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="119"/>
+      <c r="J44" s="108"/>
       <c r="K44" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="116" t="s">
+      <c r="A45" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="116"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="126">
+      <c r="B45" s="103"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="102">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D44),"")</f>
         <v>0</v>
       </c>
-      <c r="E45" s="126"/>
+      <c r="E45" s="102"/>
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="116" t="s">
+      <c r="A46" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="116"/>
-      <c r="C46" s="116"/>
-      <c r="D46" s="104">
+      <c r="B46" s="103"/>
+      <c r="C46" s="103"/>
+      <c r="D46" s="110">
         <v>5</v>
       </c>
-      <c r="E46" s="104"/>
+      <c r="E46" s="110"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="116" t="s">
+      <c r="A47" s="103" t="s">
         <v>385</v>
       </c>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="104">
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="110">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E47" s="104"/>
+      <c r="E47" s="110"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="116" t="s">
+      <c r="A48" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="104">
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="110">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E48" s="104"/>
+      <c r="E48" s="110"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D49" s="128">
+      <c r="D49" s="111">
         <f>SUM(D44:D48)</f>
         <v>50</v>
       </c>
-      <c r="E49" s="128"/>
+      <c r="E49" s="111"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
@@ -4605,20 +4623,20 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="131" t="s">
+      <c r="A53" s="109" t="s">
         <v>388</v>
       </c>
-      <c r="B53" s="131"/>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="131"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="131"/>
-      <c r="H53" s="131"/>
-      <c r="I53" s="131"/>
-      <c r="J53" s="131"/>
-      <c r="K53" s="131"/>
-      <c r="L53" s="131"/>
+      <c r="B53" s="109"/>
+      <c r="C53" s="109"/>
+      <c r="D53" s="109"/>
+      <c r="E53" s="109"/>
+      <c r="F53" s="109"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="109"/>
+      <c r="J53" s="109"/>
+      <c r="K53" s="109"/>
+      <c r="L53" s="109"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="71" t="s">
@@ -4636,38 +4654,38 @@
       <c r="L54" s="88"/>
     </row>
     <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="113" t="s">
+      <c r="A55" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="113"/>
-      <c r="C55" s="113" t="s">
+      <c r="B55" s="105"/>
+      <c r="C55" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="113"/>
-      <c r="E55" s="113" t="s">
+      <c r="D55" s="105"/>
+      <c r="E55" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="F55" s="113"/>
-      <c r="G55" s="113" t="s">
+      <c r="F55" s="105"/>
+      <c r="G55" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="113"/>
+      <c r="H55" s="105"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="129">
+      <c r="A56" s="106">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B56" s="129"/>
-      <c r="C56" s="130"/>
-      <c r="D56" s="130"/>
-      <c r="E56" s="130"/>
-      <c r="F56" s="130"/>
-      <c r="G56" s="119">
+      <c r="B56" s="106"/>
+      <c r="C56" s="107"/>
+      <c r="D56" s="107"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="107"/>
+      <c r="G56" s="108">
         <f>SUM(C56*E56)</f>
         <v>0</v>
       </c>
-      <c r="H56" s="119"/>
+      <c r="H56" s="108"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
@@ -4688,61 +4706,61 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="115" t="s">
+      <c r="A60" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="115"/>
-      <c r="C60" s="115"/>
-      <c r="D60" s="125" t="s">
+      <c r="B60" s="99"/>
+      <c r="C60" s="99"/>
+      <c r="D60" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="125"/>
+      <c r="E60" s="100"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="123" t="s">
+      <c r="A61" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="123"/>
-      <c r="C61" s="123"/>
-      <c r="D61" s="126">
+      <c r="B61" s="101"/>
+      <c r="C61" s="101"/>
+      <c r="D61" s="102">
         <f>IF(C56="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G56)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G56)))</f>
         <v>12</v>
       </c>
-      <c r="E61" s="126"/>
+      <c r="E61" s="102"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="123" t="s">
+      <c r="A62" s="101" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="123"/>
-      <c r="C62" s="123"/>
-      <c r="D62" s="126" t="str">
+      <c r="B62" s="101"/>
+      <c r="C62" s="101"/>
+      <c r="D62" s="102" t="str">
         <f>IFERROR((IF(SUM(12-D61)=0,"-",SUM(12-D61))),"")</f>
         <v>-</v>
       </c>
-      <c r="E62" s="126"/>
+      <c r="E62" s="102"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="116" t="s">
+      <c r="A63" s="103" t="s">
         <v>393</v>
       </c>
-      <c r="B63" s="116"/>
-      <c r="C63" s="116"/>
-      <c r="D63" s="132">
+      <c r="B63" s="103"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="104">
         <v>37.5</v>
       </c>
-      <c r="E63" s="132"/>
+      <c r="E63" s="104"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="116" t="s">
+      <c r="A64" s="103" t="s">
         <v>394</v>
       </c>
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="132">
+      <c r="B64" s="103"/>
+      <c r="C64" s="103"/>
+      <c r="D64" s="104">
         <v>25.5</v>
       </c>
-      <c r="E64" s="132"/>
+      <c r="E64" s="104"/>
       <c r="F64" s="5" t="s">
         <v>55</v>
       </c>
@@ -4754,75 +4772,75 @@
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="134"/>
-      <c r="D67" s="134"/>
+      <c r="B67" s="95"/>
+      <c r="C67" s="97"/>
+      <c r="D67" s="97"/>
       <c r="E67" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="96" t="s">
+      <c r="A68" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="96"/>
-      <c r="C68" s="133"/>
-      <c r="D68" s="133"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="96" t="s">
+      <c r="A69" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="96"/>
-      <c r="C69" s="133"/>
-      <c r="D69" s="133"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="96"/>
+      <c r="D69" s="96"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="135" t="str">
+      <c r="B70" s="95"/>
+      <c r="C70" s="98" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D70" s="135"/>
+      <c r="D70" s="98"/>
       <c r="E70" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="96" t="s">
+      <c r="A71" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="96"/>
-      <c r="C71" s="134"/>
-      <c r="D71" s="134"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="97"/>
+      <c r="D71" s="97"/>
       <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="96" t="s">
+      <c r="A72" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="96"/>
-      <c r="C72" s="133"/>
-      <c r="D72" s="133"/>
+      <c r="B72" s="95"/>
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
       <c r="E72" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="96"/>
-      <c r="C73" s="133"/>
-      <c r="D73" s="133"/>
+      <c r="B73" s="95"/>
+      <c r="C73" s="96"/>
+      <c r="D73" s="96"/>
       <c r="E73" s="9" t="s">
         <v>68</v>
       </c>
@@ -4830,6 +4848,108 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="116">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="A73:B73"/>
@@ -4844,157 +4964,55 @@
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="C71:D71"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B59">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>COUNTIF(B59,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4 C7:C8 F16 B39:C39 B42 C56:E56 C67:C69 C71:C73">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="14" priority="10">
       <formula>COUNTIF(B2,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12 A34">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>COUNTIF(A11,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>COUNTIF(C34,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>COUNTIF(C52,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
       <formula>800</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThanOrEqual">
       <formula>800</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="lessThan">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:G34">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>COUNTIF(E34,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>COUNTIF(F42,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5141,7 +5159,7 @@
   <dimension ref="A1:AF111"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15306,9 +15324,9 @@
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:AF1"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="D1:J98 L3:L98">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>COUNTIF(D1,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15328,6 +15346,24 @@
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="between" id="{B6EFD0E3-BE59-4DA2-8B29-4FB56BB5907C}">
+            <xm:f>0</xm:f>
+            <xm:f>reference!$B$7</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC00000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>K3:K98</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F1E3D491-2C2B-4D8B-8E3A-EF290DD37CC5}">
@@ -15350,7 +15386,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15491,14 +15527,14 @@
       <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>417</v>
-      </c>
-      <c r="C7" t="s">
-        <v>380</v>
+      <c r="A7" t="s">
+        <v>447</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" s="139" t="s">
+        <v>446</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -15509,13 +15545,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>396</v>
+        <v>417</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="E8">
         <v>50</v>
@@ -15525,16 +15561,20 @@
       <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9" t="s">
+        <v>401</v>
+      </c>
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="L9" s="35"/>
     </row>
     <row r="10" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78" t="s">
-        <v>301</v>
-      </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
       <c r="E10" s="79" t="s">
         <v>356</v>
       </c>
@@ -15543,13 +15583,12 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" t="s">
-        <v>304</v>
-      </c>
+    <row r="11" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="78" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
       <c r="E11" t="s">
         <v>58</v>
       </c>
@@ -15559,10 +15598,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
+        <v>303</v>
+      </c>
+      <c r="B12" t="s">
+        <v>304</v>
       </c>
       <c r="E12" t="s">
         <v>357</v>
@@ -15576,6 +15615,12 @@
       <c r="Q12" s="24"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
       <c r="E13" t="s">
         <v>358</v>
       </c>
@@ -15583,10 +15628,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="78" t="s">
-        <v>336</v>
-      </c>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>359</v>
       </c>
@@ -15594,14 +15636,19 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>438</v>
+    <row r="15" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="78" t="s">
+        <v>336</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>360</v>
       </c>
       <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="17" spans="5:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="79" t="s">
@@ -15803,10 +15850,10 @@
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
       <formula1>$E$23:$E$30</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{BFF87161-9E78-439F-9B63-F620B9F8A837}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{BFF87161-9E78-439F-9B63-F620B9F8A837}">
       <formula1>$E$34:$E$35</formula1>
     </dataValidation>
   </dataValidations>
@@ -15822,9 +15869,7 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>